<commit_message>
Fixed expected value computation
</commit_message>
<xml_diff>
--- a/InspectedTopWords.xlsx
+++ b/InspectedTopWords.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22880" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="22600" yWindow="0" windowWidth="27640" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
   <si>
     <t>wife</t>
   </si>
@@ -45,9 +45,18 @@
     <t>committee assignments</t>
   </si>
   <si>
+    <t>obituary</t>
+  </si>
+  <si>
+    <t>linkedin</t>
+  </si>
+  <si>
     <t>Name collision</t>
   </si>
   <si>
+    <t>actor</t>
+  </si>
+  <si>
     <t>primary</t>
   </si>
   <si>
@@ -57,9 +66,6 @@
     <t>supreme court</t>
   </si>
   <si>
-    <t>family</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -123,6 +129,12 @@
     <t>cuba</t>
   </si>
   <si>
+    <t>married</t>
+  </si>
+  <si>
+    <t>pronunciation</t>
+  </si>
+  <si>
     <t>Hypothetical Reason</t>
   </si>
   <si>
@@ -135,12 +147,6 @@
     <t>Republicans skew male</t>
   </si>
   <si>
-    <t>Male as "head of household"?</t>
-  </si>
-  <si>
-    <t>Male tendency to hold wealth?</t>
-  </si>
-  <si>
     <t>More "generic" male names? Same with name collision?</t>
   </si>
   <si>
@@ -178,13 +184,121 @@
   </si>
   <si>
     <t>israel</t>
+  </si>
+  <si>
+    <t>Republican</t>
+  </si>
+  <si>
+    <t>trump</t>
+  </si>
+  <si>
+    <t>Seems to be some administrative position in a congressional office</t>
+  </si>
+  <si>
+    <t>Harry Reid had some comments on Trump</t>
+  </si>
+  <si>
+    <t>phone number</t>
+  </si>
+  <si>
+    <t>voting record</t>
+  </si>
+  <si>
+    <t>rubio</t>
+  </si>
+  <si>
+    <t>photography</t>
+  </si>
+  <si>
+    <t>This seems like the biggest story</t>
+  </si>
+  <si>
+    <t>Black Caucus</t>
+  </si>
+  <si>
+    <t>sorority</t>
+  </si>
+  <si>
+    <t>delta sigma theta</t>
+  </si>
+  <si>
+    <t>hats</t>
+  </si>
+  <si>
+    <t>songs</t>
+  </si>
+  <si>
+    <t>missouri</t>
+  </si>
+  <si>
+    <t>football</t>
+  </si>
+  <si>
+    <t>Non Black Caucus</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>senate</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>iran</t>
+  </si>
+  <si>
+    <t>wiki</t>
+  </si>
+  <si>
+    <t>campaign</t>
+  </si>
+  <si>
+    <t>immigration</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Rejected for name collsion:</t>
+  </si>
+  <si>
+    <t>Most popular female name %</t>
+  </si>
+  <si>
+    <t>Most popular male name %</t>
+  </si>
+  <si>
+    <t>http://names.mongabay.com/female_names.htm</t>
+  </si>
+  <si>
+    <t>None of the rest of these are statistically significant</t>
+  </si>
+  <si>
+    <t>artist</t>
+  </si>
+  <si>
+    <t>Rejected for sample size:</t>
+  </si>
+  <si>
+    <t>delta signma theta</t>
+  </si>
+  <si>
+    <t>baby</t>
+  </si>
+  <si>
+    <t>campaign manager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -216,6 +330,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -234,7 +355,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -250,12 +371,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -263,6 +390,8 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -270,6 +399,8 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -599,29 +730,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K41"/>
+  <dimension ref="A3:X86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="7" max="7" width="21.83203125" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:24">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>434</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="L3" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -635,19 +770,22 @@
         <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>38</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -664,17 +802,23 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>92239.891180799998</v>
+        <v>182.529940977</v>
       </c>
       <c r="H5">
         <f>1/G5</f>
-        <v>1.084129639788813E-5</v>
+        <v>5.4785532425390242E-3</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -691,19 +835,22 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>204.39031831200001</v>
+        <v>18.949877262800001</v>
       </c>
       <c r="H6">
         <f>1/G6</f>
-        <v>4.8925996507990606E-3</v>
+        <v>5.277079033979145E-2</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>40</v>
+      </c>
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>1.84331797235E-2</v>
@@ -718,17 +865,23 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>39.346996507599997</v>
+        <v>6.3187563209900004</v>
       </c>
       <c r="H7">
         <f>1/G7</f>
-        <v>2.5414900469133566E-2</v>
+        <v>0.15825899104197827</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>41</v>
+      </c>
+      <c r="L7" t="s">
+        <v>86</v>
+      </c>
+      <c r="V7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -745,19 +898,19 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>34.100004777300001</v>
+        <v>9.4490591251199998</v>
       </c>
       <c r="H8">
         <f>1/G8</f>
-        <v>2.9325509088071713E-2</v>
+        <v>0.1058306426871152</v>
       </c>
       <c r="I8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="B9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>1.6129032258100001E-2</v>
@@ -772,148 +925,77 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>27.355121940899998</v>
+        <v>5.3506330028400004</v>
       </c>
       <c r="H9">
         <f>1/G9</f>
-        <v>3.6556225271467367E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>2.2998805256899998E-2</v>
-      </c>
-      <c r="D10">
-        <v>14</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>15.835044076499999</v>
-      </c>
-      <c r="H10">
-        <f>1/G10</f>
-        <v>6.3151071457012875E-2</v>
-      </c>
-      <c r="I10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11">
-        <v>1.8390510326E-2</v>
-      </c>
-      <c r="D11">
-        <v>12</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>8.6909149570299995</v>
-      </c>
-      <c r="H11">
-        <f>1/G11</f>
-        <v>0.11506268384217813</v>
-      </c>
-      <c r="I11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12">
-        <v>2.5217613927300001E-2</v>
-      </c>
-      <c r="D12">
-        <v>23</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>6.9394669318100002</v>
-      </c>
-      <c r="H12">
-        <f>1/G12</f>
-        <v>0.14410328773469247</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <v>2.9612561870600001E-2</v>
-      </c>
-      <c r="D13">
-        <v>45</v>
-      </c>
-      <c r="E13">
-        <v>8</v>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>4.0389562233099996</v>
-      </c>
-      <c r="H13">
-        <f>1/G13</f>
-        <v>0.24758871963719414</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14">
-        <v>2.7351083802699998E-2</v>
-      </c>
-      <c r="D14">
-        <v>40</v>
-      </c>
-      <c r="E14">
-        <v>7</v>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>3.9095497629599998</v>
-      </c>
-      <c r="H14">
-        <f>1/G14</f>
-        <v>0.25578392925810456</v>
-      </c>
-      <c r="I14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>0.18689377489901132</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="V10">
+        <v>2.629</v>
+      </c>
+      <c r="X10">
+        <v>3.3180000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="L11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V11">
+        <v>1.073</v>
+      </c>
+      <c r="X11">
+        <v>3.2709999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="L12" t="s">
+        <v>67</v>
+      </c>
+      <c r="V12">
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="X12">
+        <v>3.1429999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="L13" t="s">
+        <v>88</v>
+      </c>
+      <c r="V13">
+        <v>0.98</v>
+      </c>
+      <c r="X13">
+        <v>2.629</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="L14" t="s">
+        <v>89</v>
+      </c>
+      <c r="V14">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="X14">
+        <v>2.4510000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C15">
         <v>7.4074074074099994E-2</v>
@@ -928,19 +1010,28 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>134228.58828600001</v>
+        <v>70002132.604000002</v>
       </c>
       <c r="H15">
         <f>1/G15</f>
-        <v>7.4499777787225643E-6</v>
+        <v>1.4285279073667233E-8</v>
       </c>
       <c r="I15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>39</v>
+      </c>
+      <c r="L15" t="s">
+        <v>65</v>
+      </c>
+      <c r="V15">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="X15">
+        <v>2.363</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="B16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>8.5509472606199996E-2</v>
@@ -954,18 +1045,27 @@
       <c r="F16" t="b">
         <v>0</v>
       </c>
-      <c r="G16">
-        <v>23231.435765800001</v>
-      </c>
-      <c r="H16">
+      <c r="H16" t="e">
         <f>1/G16</f>
-        <v>4.304512256931374E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L16" t="s">
+        <v>90</v>
+      </c>
+      <c r="V16" s="1">
+        <f>SUM(V10:V15)</f>
+        <v>7.5860000000000012</v>
+      </c>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1">
+        <f>SUM(X10:X15)</f>
+        <v>17.175000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>0.17434715821800001</v>
@@ -980,22 +1080,25 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>23231.435765800001</v>
+        <v>4349.1771987299999</v>
       </c>
       <c r="H17">
         <f>1/G17</f>
-        <v>4.304512256931374E-5</v>
+        <v>2.2992854839117829E-4</v>
       </c>
       <c r="I17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>30</v>
+      </c>
+      <c r="L17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="B18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>0.141961085509</v>
@@ -1010,19 +1113,22 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>1550.18462903</v>
+        <v>387.555454811</v>
       </c>
       <c r="H18">
         <f>1/G18</f>
-        <v>6.4508445076360481E-4</v>
+        <v>2.5802759000971157E-3</v>
       </c>
       <c r="I18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>50</v>
+      </c>
+      <c r="L18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="B19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>0.20579450418199999</v>
@@ -1037,17 +1143,17 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>771.92298861799998</v>
+        <v>156.3130572</v>
       </c>
       <c r="H19">
         <f>1/G19</f>
-        <v>1.2954660176533077E-3</v>
+        <v>6.3974182190072344E-3</v>
       </c>
       <c r="I19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="B20">
         <v>2016</v>
       </c>
@@ -1061,19 +1167,19 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>737.54145294299997</v>
+        <v>2234.9877297399998</v>
       </c>
       <c r="H20">
         <f>1/G20</f>
-        <v>1.3558559942762755E-3</v>
+        <v>4.4742974947622278E-4</v>
       </c>
       <c r="I20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="B21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21">
         <v>7</v>
@@ -1085,19 +1191,19 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>362.33005385199999</v>
+        <v>454.44544024099997</v>
       </c>
       <c r="H21">
         <f>1/G21</f>
-        <v>2.7599145844205003E-3</v>
+        <v>2.2004841757674661E-3</v>
       </c>
       <c r="I21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="B22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -1109,19 +1215,19 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>164.59604056800001</v>
+        <v>1936.5487168300001</v>
       </c>
       <c r="H22">
         <f>1/G22</f>
-        <v>6.0754802882810981E-3</v>
+        <v>5.1638256828205836E-4</v>
       </c>
       <c r="I22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="B23" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D23">
         <v>6</v>
@@ -1140,12 +1246,12 @@
         <v>9.1050751538819686E-3</v>
       </c>
       <c r="I23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="B24" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>0.15962621607800001</v>
@@ -1159,20 +1265,17 @@
       <c r="F24" t="b">
         <v>0</v>
       </c>
-      <c r="G24">
-        <v>77.204475506099996</v>
-      </c>
-      <c r="H24">
+      <c r="H24" t="e">
         <f>1/G24</f>
-        <v>1.2952616975177677E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="I24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="B25" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D25">
         <v>7</v>
@@ -1183,20 +1286,17 @@
       <c r="F25" t="b">
         <v>0</v>
       </c>
-      <c r="G25">
-        <v>76.277699166700003</v>
-      </c>
-      <c r="H25">
+      <c r="H25" t="e">
         <f>1/G25</f>
-        <v>1.3109991661056324E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="I25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="B26" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C26">
         <v>0.15365250042699999</v>
@@ -1210,17 +1310,14 @@
       <c r="F26" t="b">
         <v>0</v>
       </c>
-      <c r="G26">
-        <v>24.412435353799999</v>
-      </c>
-      <c r="H26">
+      <c r="H26" t="e">
         <f>1/G26</f>
-        <v>4.0962730080280237E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="B27" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C27">
         <v>0.100913125107</v>
@@ -1234,17 +1331,14 @@
       <c r="F27" t="b">
         <v>0</v>
       </c>
-      <c r="G27">
-        <v>21.572404160200001</v>
-      </c>
-      <c r="H27">
+      <c r="H27" t="e">
         <f>1/G27</f>
-        <v>4.6355519420730566E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="B28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C28">
         <v>0.142046424304</v>
@@ -1258,20 +1352,17 @@
       <c r="F28" t="b">
         <v>0</v>
       </c>
-      <c r="G28">
-        <v>17.628239530199998</v>
-      </c>
-      <c r="H28">
+      <c r="H28" t="e">
         <f>1/G28</f>
-        <v>5.672716202243791E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="I28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="B29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C29">
         <v>8.9435057176999996E-2</v>
@@ -1285,23 +1376,20 @@
       <c r="F29" t="b">
         <v>0</v>
       </c>
-      <c r="G29">
-        <v>11.923233309800001</v>
-      </c>
-      <c r="H29">
+      <c r="H29" t="e">
         <f>1/G29</f>
-        <v>8.3869867679103052E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="I29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D34">
         <v>66</v>
@@ -1313,16 +1401,19 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <v>16207.2971452</v>
+        <v>21416.988187700001</v>
       </c>
       <c r="H34">
         <f>1/G34</f>
-        <v>6.170060257679442E-5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>4.6691906034402652E-5</v>
+      </c>
+      <c r="I34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="B35" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D35">
         <v>13</v>
@@ -1334,16 +1425,16 @@
         <v>0</v>
       </c>
       <c r="G35">
-        <v>8020.7001438300003</v>
+        <v>19926.9822914</v>
       </c>
       <c r="H35">
-        <f t="shared" ref="H35:H41" si="0">1/G35</f>
-        <v>1.2467739499889664E-4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <f t="shared" ref="H35:H49" si="0">1/G35</f>
+        <v>5.0183213161762862E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="B36" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D36">
         <v>12</v>
@@ -1355,16 +1446,16 @@
         <v>0</v>
       </c>
       <c r="G36">
-        <v>4393.5283630200001</v>
+        <v>10212.8422538</v>
       </c>
       <c r="H36">
         <f t="shared" si="0"/>
-        <v>2.2760749843267776E-4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>9.7915935167599351E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="B37" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D37">
         <v>9</v>
@@ -1372,17 +1463,23 @@
       <c r="E37">
         <v>0</v>
       </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
       <c r="G37">
-        <v>708.64562939400003</v>
+        <v>1348.7061188800001</v>
       </c>
       <c r="H37">
         <f t="shared" si="0"/>
-        <v>1.4111425492811581E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>7.4145137031811305E-4</v>
+      </c>
+      <c r="I37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="B38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D38">
         <v>14</v>
@@ -1394,16 +1491,16 @@
         <v>0</v>
       </c>
       <c r="G38">
-        <v>448.82389040300001</v>
+        <v>659.51471604400001</v>
       </c>
       <c r="H38">
         <f t="shared" si="0"/>
-        <v>2.2280453901464508E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>1.5162663935663935E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="B39" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D39">
         <v>12</v>
@@ -1415,16 +1512,16 @@
         <v>0</v>
       </c>
       <c r="G39">
-        <v>63.551104552300004</v>
+        <v>77.094611647700006</v>
       </c>
       <c r="H39">
         <f t="shared" si="0"/>
-        <v>1.5735367733491403E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>1.2971075132587861E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="B40" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D40">
         <v>4</v>
@@ -1436,16 +1533,16 @@
         <v>0</v>
       </c>
       <c r="G40">
-        <v>30.014646015099999</v>
+        <v>40.8148861588</v>
       </c>
       <c r="H40">
         <f t="shared" si="0"/>
-        <v>3.3317067924003248E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>2.4500864613691747E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="B41" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D41">
         <v>4</v>
@@ -1457,11 +1554,654 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>30.014646015099999</v>
+        <v>40.8148861588</v>
       </c>
       <c r="H41">
         <f t="shared" si="0"/>
-        <v>3.3317067924003248E-2</v>
+        <v>2.4500864613691747E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42">
+        <v>23</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>12539.9444358</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>7.9745169934335825E-5</v>
+      </c>
+      <c r="I42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43">
+        <v>13</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>743.23048311299999</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>1.345477644850529E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44">
+        <v>40</v>
+      </c>
+      <c r="E44">
+        <v>13</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>249.50530092899999</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>4.0079308787293591E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45">
+        <v>20</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>66.643996215300007</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="0"/>
+        <v>1.5005102586726661E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="B46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46">
+        <v>7</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>53.645178920799999</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="0"/>
+        <v>1.8641004096125163E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47">
+        <v>38</v>
+      </c>
+      <c r="E47">
+        <v>15</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>49.728274775199999</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="0"/>
+        <v>2.0109283994278245E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48">
+        <v>5</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>21.3792568876</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="0"/>
+        <v>4.6774310503748209E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="B49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49">
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>21.3792568876</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="0"/>
+        <v>4.6774310503748209E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54">
+        <v>5</v>
+      </c>
+      <c r="E54">
+        <v>8</v>
+      </c>
+      <c r="G54">
+        <v>62117.036675900003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="1"/>
+      <c r="B55" t="s">
+        <v>65</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>1672.6144026500001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="B56" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>1672.6144026500001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="B57" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>1672.6144026500001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="B58" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>5</v>
+      </c>
+      <c r="G58">
+        <v>1063.3154804400001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="B59" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>727.79310185600002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="B60" t="s">
+        <v>51</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="E60">
+        <v>6</v>
+      </c>
+      <c r="G60">
+        <v>602.05849959</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="B61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="G61">
+        <v>345.964830818</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="B62" t="s">
+        <v>54</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="G62">
+        <v>345.964830818</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="B63" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="G63">
+        <v>177.70821317400001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64">
+        <v>11</v>
+      </c>
+      <c r="E64">
+        <v>68</v>
+      </c>
+      <c r="G64">
+        <v>161.991378475</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="B65" t="s">
+        <v>34</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65">
+        <v>9</v>
+      </c>
+      <c r="G65">
+        <v>137.415271795</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="B66" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66">
+        <v>20</v>
+      </c>
+      <c r="E66">
+        <v>152</v>
+      </c>
+      <c r="G66">
+        <v>70.742824153599997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="B67" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67">
+        <v>7</v>
+      </c>
+      <c r="E67">
+        <v>40</v>
+      </c>
+      <c r="G67">
+        <v>68.156340598</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" t="s">
+        <v>72</v>
+      </c>
+      <c r="D68">
+        <v>28</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>10893.8566937</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="B69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69">
+        <v>26</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>6102.0951852799999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="B70" t="s">
+        <v>73</v>
+      </c>
+      <c r="D70">
+        <v>25</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>4562.9556514300002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="B71" t="s">
+        <v>74</v>
+      </c>
+      <c r="D71">
+        <v>44</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>1100.3043413</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="B72" t="s">
+        <v>52</v>
+      </c>
+      <c r="D72">
+        <v>17</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>433.61134612199999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="B73" t="s">
+        <v>75</v>
+      </c>
+      <c r="D73">
+        <v>16</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>321.57001321000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="B74" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74">
+        <v>16</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>321.57001321000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="B75" t="s">
+        <v>28</v>
+      </c>
+      <c r="D75">
+        <v>13</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>129.93313932199999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="B76" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76">
+        <v>13</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>129.93313932199999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="B77" t="s">
+        <v>60</v>
+      </c>
+      <c r="D77">
+        <v>51</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="G77">
+        <v>93.933587104400004</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="B78" t="s">
+        <v>76</v>
+      </c>
+      <c r="D78">
+        <v>11</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>70.301846759200004</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="B79" t="s">
+        <v>77</v>
+      </c>
+      <c r="D79">
+        <v>106</v>
+      </c>
+      <c r="E79">
+        <v>6</v>
+      </c>
+      <c r="G79">
+        <v>51.420010564899997</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+      <c r="D80">
+        <v>259</v>
+      </c>
+      <c r="E80">
+        <v>18</v>
+      </c>
+      <c r="G80">
+        <v>41.3462003307</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7">
+      <c r="B81">
+        <v>2016</v>
+      </c>
+      <c r="D81">
+        <v>9</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>37.610324992499997</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7">
+      <c r="B82" t="s">
+        <v>27</v>
+      </c>
+      <c r="D82">
+        <v>8</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>27.355121940899998</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7">
+      <c r="B83" t="s">
+        <v>78</v>
+      </c>
+      <c r="D83">
+        <v>8</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>27.355121940899998</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7">
+      <c r="B84" t="s">
+        <v>79</v>
+      </c>
+      <c r="D84">
+        <v>8</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>27.355121940899998</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7">
+      <c r="B85" t="s">
+        <v>80</v>
+      </c>
+      <c r="D85">
+        <v>8</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>27.355121940899998</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7">
+      <c r="B86" t="s">
+        <v>19</v>
+      </c>
+      <c r="D86">
+        <v>363</v>
+      </c>
+      <c r="E86">
+        <v>27</v>
+      </c>
+      <c r="G86">
+        <v>26.460160586800001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added within-gender party comparison, culled low sample size terms
</commit_message>
<xml_diff>
--- a/InspectedTopWords.xlsx
+++ b/InspectedTopWords.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22600" yWindow="0" windowWidth="27640" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="27220" yWindow="0" windowWidth="27640" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
   <si>
     <t>wife</t>
   </si>
@@ -81,21 +81,12 @@
     <t>staff</t>
   </si>
   <si>
-    <t>twitter</t>
-  </si>
-  <si>
     <t>internship</t>
   </si>
   <si>
     <t>chief staff</t>
   </si>
   <si>
-    <t>facebook</t>
-  </si>
-  <si>
-    <t>for congress</t>
-  </si>
-  <si>
     <t>husband</t>
   </si>
   <si>
@@ -165,9 +156,6 @@
     <t>Dems skew female, Cuba an Obama initiative?</t>
   </si>
   <si>
-    <t>More interest in life stories of underrepresented groups? Dems skew female and tend to be more internet savvy?</t>
-  </si>
-  <si>
     <t>Democrat</t>
   </si>
   <si>
@@ -292,6 +280,18 @@
   </si>
   <si>
     <t>campaign manager</t>
+  </si>
+  <si>
+    <t>vice president</t>
+  </si>
+  <si>
+    <t>poll</t>
+  </si>
+  <si>
+    <t>% Matching</t>
+  </si>
+  <si>
+    <t>% Other</t>
   </si>
 </sst>
 </file>
@@ -355,8 +355,120 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -382,7 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="131">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -392,6 +504,62 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -401,6 +569,62 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -732,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:X86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -741,8 +965,8 @@
     <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:24">
@@ -752,8 +976,8 @@
       <c r="B3">
         <v>434</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>81</v>
+      <c r="N3" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -767,21 +991,27 @@
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -796,28 +1026,36 @@
         <v>31</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="b">
+        <f>D5/$B$3 * 100</f>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
+        <f>F5/$B$14 * 100</f>
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>182.529940977</v>
       </c>
-      <c r="H5">
-        <f>1/G5</f>
+      <c r="J5">
+        <f>1/I5</f>
         <v>5.4785532425390242E-3</v>
       </c>
-      <c r="I5" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:24">
       <c r="A6" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -829,28 +1067,36 @@
         <v>30</v>
       </c>
       <c r="E6">
+        <f t="shared" ref="E6:E9" si="0">D6/$B$3 * 100</f>
+        <v>6.9124423963133648</v>
+      </c>
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
       <c r="G6">
+        <f t="shared" ref="G6:G9" si="1">F6/$B$14 * 100</f>
+        <v>1.8518518518518516</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>18.949877262800001</v>
       </c>
-      <c r="H6">
-        <f>1/G6</f>
+      <c r="J6">
+        <f>1/I6</f>
         <v>5.277079033979145E-2</v>
       </c>
-      <c r="I6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:24">
       <c r="B7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>1.84331797235E-2</v>
@@ -859,26 +1105,34 @@
         <v>8</v>
       </c>
       <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="b">
+        <f t="shared" si="0"/>
+        <v>1.8433179723502304</v>
+      </c>
+      <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>6.3187563209900004</v>
       </c>
-      <c r="H7">
-        <f>1/G7</f>
+      <c r="J7">
+        <f>1/I7</f>
         <v>0.15825899104197827</v>
       </c>
-      <c r="I7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" t="s">
-        <v>86</v>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" t="s">
+        <v>82</v>
       </c>
       <c r="V7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -892,25 +1146,33 @@
         <v>69</v>
       </c>
       <c r="E8">
+        <f t="shared" si="0"/>
+        <v>15.898617511520738</v>
+      </c>
+      <c r="F8">
         <v>10</v>
       </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
       <c r="G8">
+        <f t="shared" si="1"/>
+        <v>9.2592592592592595</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>9.4490591251199998</v>
       </c>
-      <c r="H8">
-        <f>1/G8</f>
+      <c r="J8">
+        <f>1/I8</f>
         <v>0.1058306426871152</v>
       </c>
-      <c r="I8" t="s">
-        <v>42</v>
+      <c r="K8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:24">
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>1.6129032258100001E-2</v>
@@ -919,23 +1181,31 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="b">
+        <f t="shared" si="0"/>
+        <v>1.6129032258064515</v>
+      </c>
+      <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>5.3506330028400004</v>
       </c>
-      <c r="H9">
-        <f>1/G9</f>
+      <c r="J9">
+        <f>1/I9</f>
         <v>0.18689377489901132</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -947,8 +1217,8 @@
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="L11" s="1" t="s">
-        <v>87</v>
+      <c r="N11" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="V11">
         <v>1.073</v>
@@ -958,8 +1228,8 @@
       </c>
     </row>
     <row r="12" spans="1:24">
-      <c r="L12" t="s">
-        <v>67</v>
+      <c r="N12" t="s">
+        <v>63</v>
       </c>
       <c r="V12">
         <v>1.0349999999999999</v>
@@ -969,8 +1239,8 @@
       </c>
     </row>
     <row r="13" spans="1:24">
-      <c r="L13" t="s">
-        <v>88</v>
+      <c r="N13" t="s">
+        <v>84</v>
       </c>
       <c r="V13">
         <v>0.98</v>
@@ -980,8 +1250,14 @@
       </c>
     </row>
     <row r="14" spans="1:24">
-      <c r="L14" t="s">
-        <v>89</v>
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>108</v>
+      </c>
+      <c r="N14" t="s">
+        <v>85</v>
       </c>
       <c r="V14">
         <v>0.93700000000000006</v>
@@ -991,11 +1267,8 @@
       </c>
     </row>
     <row r="15" spans="1:24">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>7.4074074074099994E-2</v>
@@ -1004,23 +1277,31 @@
         <v>8</v>
       </c>
       <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="b">
+        <f>D15/$B$14 * 100</f>
+        <v>7.4074074074074066</v>
+      </c>
+      <c r="F15">
         <v>0</v>
       </c>
       <c r="G15">
+        <f>F15/$B$3 * 100</f>
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15">
         <v>70002132.604000002</v>
       </c>
-      <c r="H15">
-        <f>1/G15</f>
+      <c r="J15">
+        <f>1/I15</f>
         <v>1.4285279073667233E-8</v>
       </c>
-      <c r="I15" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" t="s">
-        <v>65</v>
+      <c r="K15" t="s">
+        <v>36</v>
+      </c>
+      <c r="N15" t="s">
+        <v>61</v>
       </c>
       <c r="V15">
         <v>0.93200000000000005</v>
@@ -1031,26 +1312,40 @@
     </row>
     <row r="16" spans="1:24">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C16">
-        <v>8.5509472606199996E-2</v>
+        <v>0.17434715821800001</v>
       </c>
       <c r="D16">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="E16">
-        <v>204</v>
-      </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" t="e">
-        <f>1/G16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16" t="s">
-        <v>90</v>
+        <f t="shared" ref="E16:E26" si="2">D16/$B$14 * 100</f>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="F16">
+        <v>69</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G26" si="3">F16/$B$3 * 100</f>
+        <v>15.898617511520738</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>4349.1771987299999</v>
+      </c>
+      <c r="J16">
+        <f>1/I16</f>
+        <v>2.2992854839117829E-4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" t="s">
+        <v>86</v>
       </c>
       <c r="V16" s="1">
         <f>SUM(V10:V15)</f>
@@ -1062,554 +1357,649 @@
         <v>17.175000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:14">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C17">
-        <v>0.17434715821800001</v>
+        <v>0.141961085509</v>
       </c>
       <c r="D17">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E17">
+        <f t="shared" si="2"/>
+        <v>30.555555555555557</v>
+      </c>
+      <c r="F17">
+        <v>71</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>16.359447004608295</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>387.555454811</v>
+      </c>
+      <c r="J17">
+        <f>1/I17</f>
+        <v>2.5802759000971157E-3</v>
+      </c>
+      <c r="K17" t="s">
+        <v>46</v>
+      </c>
+      <c r="M17" t="s">
+        <v>27</v>
+      </c>
+      <c r="N17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>0.20579450418199999</v>
+      </c>
+      <c r="D18">
+        <v>71</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>65.740740740740748</v>
+      </c>
+      <c r="F18">
+        <v>196</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>45.161290322580641</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>156.3130572</v>
+      </c>
+      <c r="J18">
+        <f>1/I18</f>
+        <v>6.3974182190072344E-3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="B19">
+        <v>2016</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>5.5555555555555554</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>0.69124423963133641</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>2234.9877297399998</v>
+      </c>
+      <c r="J19">
+        <f>1/I19</f>
+        <v>4.4742974947622278E-4</v>
+      </c>
+      <c r="K19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>6.481481481481481</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>1.3824884792626728</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>454.44544024099997</v>
+      </c>
+      <c r="J20">
+        <f>1/I20</f>
+        <v>2.2004841757674661E-3</v>
+      </c>
+      <c r="K20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>1936.5487168300001</v>
+      </c>
+      <c r="J21">
+        <f>1/I21</f>
+        <v>5.1638256828205836E-4</v>
+      </c>
+      <c r="K21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>5.5555555555555554</v>
+      </c>
+      <c r="F22">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>1.3824884792626728</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>109.828857324</v>
+      </c>
+      <c r="J22">
+        <f>1/I22</f>
+        <v>9.1050751538819686E-3</v>
+      </c>
+      <c r="K22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>0.15962621607800001</v>
+      </c>
+      <c r="D23">
         <v>69</v>
       </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>4349.1771987299999</v>
-      </c>
-      <c r="H17">
-        <f>1/G17</f>
-        <v>2.2992854839117829E-4</v>
-      </c>
-      <c r="I17" t="s">
-        <v>43</v>
-      </c>
-      <c r="K17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>63.888888888888886</v>
+      </c>
+      <c r="F23">
+        <v>208</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>47.926267281105986</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>26.418314666600001</v>
+      </c>
+      <c r="J23">
+        <f>1/I23</f>
+        <v>3.7852528165404679E-2</v>
+      </c>
+      <c r="K23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18">
-        <v>0.141961085509</v>
-      </c>
-      <c r="D18">
-        <v>33</v>
-      </c>
-      <c r="E18">
-        <v>71</v>
-      </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>387.555454811</v>
-      </c>
-      <c r="H18">
-        <f>1/G18</f>
-        <v>2.5802759000971157E-3</v>
-      </c>
-      <c r="I18" t="s">
+    <row r="24" spans="1:14">
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24">
+        <v>7</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>6.481481481481481</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>2.0737327188940093</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>58.6605817433</v>
+      </c>
+      <c r="J24">
+        <f>1/I24</f>
+        <v>1.7047222688244417E-2</v>
+      </c>
+      <c r="K24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>0.46082949308755761</v>
+      </c>
+      <c r="I25">
+        <v>40.197394443599997</v>
+      </c>
+      <c r="J25">
+        <f>1/I25</f>
+        <v>2.4877234304404385E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>0.46082949308755761</v>
+      </c>
+      <c r="I26">
+        <v>40.197394443599997</v>
+      </c>
+      <c r="J26">
+        <f>1/I26</f>
+        <v>2.4877234304404385E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33">
+        <v>66</v>
+      </c>
+      <c r="E33">
+        <f>D33/$B$32 * 100</f>
+        <v>28.448275862068968</v>
+      </c>
+      <c r="F33">
+        <v>37</v>
+      </c>
+      <c r="G33">
+        <f>F33/$B$41 * 100</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>21416.988187700001</v>
+      </c>
+      <c r="J33">
+        <f>1/I33</f>
+        <v>4.6691906034402652E-5</v>
+      </c>
+      <c r="K33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34">
+        <v>13</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E40" si="4">D34/$B$32 * 100</f>
+        <v>5.6034482758620694</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" ref="G34:G40" si="5">F34/$B$41 * 100</f>
+        <v>0</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>19926.9822914</v>
+      </c>
+      <c r="J34">
+        <f>1/I34</f>
+        <v>5.0183213161762862E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35">
+        <v>12</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="4"/>
+        <v>5.1724137931034484</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>10212.8422538</v>
+      </c>
+      <c r="J35">
+        <f>1/I35</f>
+        <v>9.7915935167599351E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36">
+        <v>9</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="4"/>
+        <v>3.8793103448275863</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>1348.7061188800001</v>
+      </c>
+      <c r="J36">
+        <f>1/I36</f>
+        <v>7.4145137031811305E-4</v>
+      </c>
+      <c r="K36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37">
+        <v>14</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="4"/>
+        <v>6.0344827586206895</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>659.51471604400001</v>
+      </c>
+      <c r="J37">
+        <f>1/I37</f>
+        <v>1.5162663935663935E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38">
+        <v>12</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="4"/>
+        <v>5.1724137931034484</v>
+      </c>
+      <c r="F38">
+        <v>4</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="5"/>
+        <v>1.3333333333333335</v>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>77.094611647700006</v>
+      </c>
+      <c r="J38">
+        <f>1/I38</f>
+        <v>1.2971075132587861E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="4"/>
+        <v>1.7241379310344827</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>40.8148861588</v>
+      </c>
+      <c r="J39">
+        <f>1/I39</f>
+        <v>2.4500864613691747E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="B40" t="s">
         <v>50</v>
-      </c>
-      <c r="L18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19">
-        <v>0.20579450418199999</v>
-      </c>
-      <c r="D19">
-        <v>71</v>
-      </c>
-      <c r="E19">
-        <v>196</v>
-      </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>156.3130572</v>
-      </c>
-      <c r="H19">
-        <f>1/G19</f>
-        <v>6.3974182190072344E-3</v>
-      </c>
-      <c r="I19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="B20">
-        <v>2016</v>
-      </c>
-      <c r="D20">
-        <v>6</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>2234.9877297399998</v>
-      </c>
-      <c r="H20">
-        <f>1/G20</f>
-        <v>4.4742974947622278E-4</v>
-      </c>
-      <c r="I20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21">
-        <v>7</v>
-      </c>
-      <c r="E21">
-        <v>6</v>
-      </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>454.44544024099997</v>
-      </c>
-      <c r="H21">
-        <f>1/G21</f>
-        <v>2.2004841757674661E-3</v>
-      </c>
-      <c r="I21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="B22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" t="b">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>1936.5487168300001</v>
-      </c>
-      <c r="H22">
-        <f>1/G22</f>
-        <v>5.1638256828205836E-4</v>
-      </c>
-      <c r="I22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="B23" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23">
-        <v>6</v>
-      </c>
-      <c r="E23">
-        <v>6</v>
-      </c>
-      <c r="F23" t="b">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>109.828857324</v>
-      </c>
-      <c r="H23">
-        <f>1/G23</f>
-        <v>9.1050751538819686E-3</v>
-      </c>
-      <c r="I23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24">
-        <v>0.15962621607800001</v>
-      </c>
-      <c r="D24">
-        <v>69</v>
-      </c>
-      <c r="E24">
-        <v>208</v>
-      </c>
-      <c r="F24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" t="e">
-        <f>1/G24</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25">
-        <v>7</v>
-      </c>
-      <c r="E25">
-        <v>9</v>
-      </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" t="e">
-        <f>1/G25</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26">
-        <v>0.15365250042699999</v>
-      </c>
-      <c r="D26">
-        <v>91</v>
-      </c>
-      <c r="E26">
-        <v>299</v>
-      </c>
-      <c r="F26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" t="e">
-        <f>1/G26</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="B27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27">
-        <v>0.100913125107</v>
-      </c>
-      <c r="D27">
-        <v>43</v>
-      </c>
-      <c r="E27">
-        <v>129</v>
-      </c>
-      <c r="F27" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" t="e">
-        <f>1/G27</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28">
-        <v>0.142046424304</v>
-      </c>
-      <c r="D28">
-        <v>89</v>
-      </c>
-      <c r="E28">
-        <v>296</v>
-      </c>
-      <c r="F28" t="b">
-        <v>0</v>
-      </c>
-      <c r="H28" t="e">
-        <f>1/G28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29">
-        <v>8.9435057176999996E-2</v>
-      </c>
-      <c r="D29">
-        <v>44</v>
-      </c>
-      <c r="E29">
-        <v>138</v>
-      </c>
-      <c r="F29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H29" t="e">
-        <f>1/G29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34">
-        <v>66</v>
-      </c>
-      <c r="E34">
-        <v>37</v>
-      </c>
-      <c r="F34" t="b">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>21416.988187700001</v>
-      </c>
-      <c r="H34">
-        <f>1/G34</f>
-        <v>4.6691906034402652E-5</v>
-      </c>
-      <c r="I34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="B35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35">
-        <v>13</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35" t="b">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>19926.9822914</v>
-      </c>
-      <c r="H35">
-        <f t="shared" ref="H35:H49" si="0">1/G35</f>
-        <v>5.0183213161762862E-5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36">
-        <v>12</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" t="b">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>10212.8422538</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="0"/>
-        <v>9.7915935167599351E-5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="B37" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37">
-        <v>9</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" t="b">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>1348.7061188800001</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="0"/>
-        <v>7.4145137031811305E-4</v>
-      </c>
-      <c r="I37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="B38" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38">
-        <v>14</v>
-      </c>
-      <c r="E38">
-        <v>3</v>
-      </c>
-      <c r="F38" t="b">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>659.51471604400001</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="0"/>
-        <v>1.5162663935663935E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="B39" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39">
-        <v>12</v>
-      </c>
-      <c r="E39">
-        <v>4</v>
-      </c>
-      <c r="F39" t="b">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>77.094611647700006</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="0"/>
-        <v>1.2971075132587861E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="B40" t="s">
-        <v>53</v>
       </c>
       <c r="D40">
         <v>4</v>
       </c>
       <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40" t="b">
+        <f t="shared" si="4"/>
+        <v>1.7241379310344827</v>
+      </c>
+      <c r="F40">
         <v>0</v>
       </c>
       <c r="G40">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40">
         <v>40.8148861588</v>
       </c>
-      <c r="H40">
-        <f t="shared" si="0"/>
+      <c r="J40">
+        <f>1/I40</f>
         <v>2.4500864613691747E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
-      <c r="B41" t="s">
-        <v>54</v>
-      </c>
-      <c r="D41">
-        <v>4</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41" t="b">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>40.8148861588</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="0"/>
-        <v>2.4500864613691747E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="1" t="s">
-        <v>55</v>
-      </c>
+    <row r="41" spans="1:11">
+      <c r="A41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="B42" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D42">
         <v>23</v>
       </c>
       <c r="E42">
+        <f>D42/$B$41 * 100</f>
+        <v>7.6666666666666661</v>
+      </c>
+      <c r="F42">
         <v>1</v>
       </c>
-      <c r="F42" t="b">
-        <v>0</v>
-      </c>
       <c r="G42">
+        <f>F42/$B$32 * 100</f>
+        <v>0.43103448275862066</v>
+      </c>
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42">
         <v>12539.9444358</v>
       </c>
-      <c r="H42">
-        <f t="shared" si="0"/>
+      <c r="J42">
+        <f t="shared" ref="J35:J49" si="6">1/I42</f>
         <v>7.9745169934335825E-5</v>
       </c>
-      <c r="I42" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="K42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="B43" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D43">
         <v>13</v>
       </c>
       <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43" t="b">
+        <f t="shared" ref="E43:E49" si="7">D43/$B$41 * 100</f>
+        <v>4.3333333333333339</v>
+      </c>
+      <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
+        <f t="shared" ref="G43:G49" si="8">F43/$B$32 * 100</f>
+        <v>0</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43">
         <v>743.23048311299999</v>
       </c>
-      <c r="H43">
-        <f t="shared" si="0"/>
+      <c r="J43">
+        <f t="shared" si="6"/>
         <v>1.345477644850529E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:11">
       <c r="B44" t="s">
         <v>12</v>
       </c>
@@ -1617,20 +2007,28 @@
         <v>40</v>
       </c>
       <c r="E44">
+        <f t="shared" si="7"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="F44">
         <v>13</v>
       </c>
-      <c r="F44" t="b">
-        <v>0</v>
-      </c>
       <c r="G44">
+        <f t="shared" si="8"/>
+        <v>5.6034482758620694</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44">
         <v>249.50530092899999</v>
       </c>
-      <c r="H44">
-        <f t="shared" si="0"/>
+      <c r="J44">
+        <f t="shared" si="6"/>
         <v>4.0079308787293591E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:11">
       <c r="B45" t="s">
         <v>14</v>
       </c>
@@ -1638,569 +2036,609 @@
         <v>20</v>
       </c>
       <c r="E45">
+        <f t="shared" si="7"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="F45">
         <v>5</v>
       </c>
-      <c r="F45" t="b">
-        <v>0</v>
-      </c>
       <c r="G45">
+        <f t="shared" si="8"/>
+        <v>2.1551724137931036</v>
+      </c>
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45">
         <v>66.643996215300007</v>
       </c>
-      <c r="H45">
-        <f t="shared" si="0"/>
+      <c r="J45">
+        <f t="shared" si="6"/>
         <v>1.5005102586726661E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:11">
       <c r="B46" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D46">
         <v>7</v>
       </c>
       <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46" t="b">
+        <f t="shared" si="7"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="F46">
         <v>0</v>
       </c>
       <c r="G46">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46">
         <v>53.645178920799999</v>
       </c>
-      <c r="H46">
-        <f t="shared" si="0"/>
+      <c r="J46">
+        <f t="shared" si="6"/>
         <v>1.8641004096125163E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:11">
       <c r="B47" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D47">
         <v>38</v>
       </c>
       <c r="E47">
+        <f t="shared" si="7"/>
+        <v>12.666666666666668</v>
+      </c>
+      <c r="F47">
         <v>15</v>
       </c>
-      <c r="F47" t="b">
-        <v>0</v>
-      </c>
       <c r="G47">
+        <f t="shared" si="8"/>
+        <v>6.4655172413793105</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47">
         <v>49.728274775199999</v>
       </c>
-      <c r="H47">
-        <f t="shared" si="0"/>
+      <c r="J47">
+        <f t="shared" si="6"/>
         <v>2.0109283994278245E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:11">
       <c r="B48" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D48">
         <v>5</v>
       </c>
       <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48" t="b">
+        <f t="shared" si="7"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F48">
         <v>0</v>
       </c>
       <c r="G48">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48">
         <v>21.3792568876</v>
       </c>
-      <c r="H48">
-        <f t="shared" si="0"/>
+      <c r="J48">
+        <f t="shared" si="6"/>
         <v>4.6774310503748209E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:10">
       <c r="B49" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D49">
         <v>5</v>
       </c>
       <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49" t="b">
+        <f t="shared" si="7"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F49">
         <v>0</v>
       </c>
       <c r="G49">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49">
         <v>21.3792568876</v>
       </c>
-      <c r="H49">
-        <f t="shared" si="0"/>
+      <c r="J49">
+        <f t="shared" si="6"/>
         <v>4.6774310503748209E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D54">
         <v>5</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>8</v>
       </c>
-      <c r="G54">
+      <c r="I54">
         <v>62117.036675900003</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:10">
       <c r="A55" s="1"/>
       <c r="B55" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D55">
         <v>2</v>
       </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="G55">
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="I55">
         <v>1672.6144026500001</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:10">
       <c r="B56" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D56">
         <v>2</v>
       </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="G56">
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="I56">
         <v>1672.6144026500001</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:10">
       <c r="B57" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D57">
         <v>2</v>
       </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="G57">
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="I57">
         <v>1672.6144026500001</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:10">
       <c r="B58" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D58">
         <v>3</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>5</v>
       </c>
-      <c r="G58">
+      <c r="I58">
         <v>1063.3154804400001</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:10">
       <c r="B59" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D59">
         <v>2</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>1</v>
       </c>
-      <c r="G59">
+      <c r="I59">
         <v>727.79310185600002</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:10">
       <c r="B60" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D60">
         <v>3</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>6</v>
       </c>
-      <c r="G60">
+      <c r="I60">
         <v>602.05849959</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:10">
       <c r="B61" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D61">
         <v>2</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>2</v>
       </c>
-      <c r="G61">
+      <c r="I61">
         <v>345.964830818</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:10">
       <c r="B62" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>2</v>
       </c>
-      <c r="G62">
+      <c r="I62">
         <v>345.964830818</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:10">
       <c r="B63" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D63">
         <v>2</v>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>3</v>
       </c>
-      <c r="G63">
+      <c r="I63">
         <v>177.70821317400001</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:10">
       <c r="B64" t="s">
         <v>6</v>
       </c>
       <c r="D64">
         <v>11</v>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>68</v>
       </c>
-      <c r="G64">
+      <c r="I64">
         <v>161.991378475</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:9">
       <c r="B65" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D65">
         <v>3</v>
       </c>
-      <c r="E65">
+      <c r="F65">
         <v>9</v>
       </c>
-      <c r="G65">
+      <c r="I65">
         <v>137.415271795</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:9">
       <c r="B66" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D66">
         <v>20</v>
       </c>
-      <c r="E66">
+      <c r="F66">
         <v>152</v>
       </c>
-      <c r="G66">
+      <c r="I66">
         <v>70.742824153599997</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:9">
       <c r="B67" t="s">
         <v>13</v>
       </c>
       <c r="D67">
         <v>7</v>
       </c>
-      <c r="E67">
+      <c r="F67">
         <v>40</v>
       </c>
-      <c r="G67">
+      <c r="I67">
         <v>68.156340598</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D68">
         <v>28</v>
       </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="G68">
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="I68">
         <v>10893.8566937</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:9">
       <c r="B69" t="s">
         <v>14</v>
       </c>
       <c r="D69">
         <v>26</v>
       </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="G69">
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="I69">
         <v>6102.0951852799999</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:9">
       <c r="B70" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D70">
         <v>25</v>
       </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="G70">
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="I70">
         <v>4562.9556514300002</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:9">
       <c r="B71" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D71">
         <v>44</v>
       </c>
-      <c r="E71">
+      <c r="F71">
         <v>1</v>
       </c>
-      <c r="G71">
+      <c r="I71">
         <v>1100.3043413</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:9">
       <c r="B72" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D72">
         <v>17</v>
       </c>
-      <c r="E72">
-        <v>0</v>
-      </c>
-      <c r="G72">
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="I72">
         <v>433.61134612199999</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:9">
       <c r="B73" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D73">
         <v>16</v>
       </c>
-      <c r="E73">
-        <v>0</v>
-      </c>
-      <c r="G73">
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="I73">
         <v>321.57001321000001</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:9">
       <c r="B74" t="s">
         <v>9</v>
       </c>
       <c r="D74">
         <v>16</v>
       </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-      <c r="G74">
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="I74">
         <v>321.57001321000001</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:9">
       <c r="B75" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D75">
         <v>13</v>
       </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="G75">
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="I75">
         <v>129.93313932199999</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:9">
       <c r="B76" t="s">
         <v>11</v>
       </c>
       <c r="D76">
         <v>13</v>
       </c>
-      <c r="E76">
-        <v>0</v>
-      </c>
-      <c r="G76">
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="I76">
         <v>129.93313932199999</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:9">
       <c r="B77" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D77">
         <v>51</v>
       </c>
-      <c r="E77">
+      <c r="F77">
         <v>2</v>
       </c>
-      <c r="G77">
+      <c r="I77">
         <v>93.933587104400004</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:9">
       <c r="B78" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D78">
         <v>11</v>
       </c>
-      <c r="E78">
-        <v>0</v>
-      </c>
-      <c r="G78">
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="I78">
         <v>70.301846759200004</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:9">
       <c r="B79" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D79">
         <v>106</v>
       </c>
-      <c r="E79">
+      <c r="F79">
         <v>6</v>
       </c>
-      <c r="G79">
+      <c r="I79">
         <v>51.420010564899997</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:9">
       <c r="B80" t="s">
         <v>18</v>
       </c>
       <c r="D80">
         <v>259</v>
       </c>
-      <c r="E80">
+      <c r="F80">
         <v>18</v>
       </c>
-      <c r="G80">
+      <c r="I80">
         <v>41.3462003307</v>
       </c>
     </row>
-    <row r="81" spans="2:7">
+    <row r="81" spans="2:9">
       <c r="B81">
         <v>2016</v>
       </c>
       <c r="D81">
         <v>9</v>
       </c>
-      <c r="E81">
-        <v>0</v>
-      </c>
-      <c r="G81">
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="I81">
         <v>37.610324992499997</v>
       </c>
     </row>
-    <row r="82" spans="2:7">
+    <row r="82" spans="2:9">
       <c r="B82" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D82">
         <v>8</v>
       </c>
-      <c r="E82">
-        <v>0</v>
-      </c>
-      <c r="G82">
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="I82">
         <v>27.355121940899998</v>
       </c>
     </row>
-    <row r="83" spans="2:7">
+    <row r="83" spans="2:9">
       <c r="B83" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D83">
         <v>8</v>
       </c>
-      <c r="E83">
-        <v>0</v>
-      </c>
-      <c r="G83">
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="I83">
         <v>27.355121940899998</v>
       </c>
     </row>
-    <row r="84" spans="2:7">
+    <row r="84" spans="2:9">
       <c r="B84" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D84">
         <v>8</v>
       </c>
-      <c r="E84">
-        <v>0</v>
-      </c>
-      <c r="G84">
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="I84">
         <v>27.355121940899998</v>
       </c>
     </row>
-    <row r="85" spans="2:7">
+    <row r="85" spans="2:9">
       <c r="B85" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D85">
         <v>8</v>
       </c>
-      <c r="E85">
-        <v>0</v>
-      </c>
-      <c r="G85">
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="I85">
         <v>27.355121940899998</v>
       </c>
     </row>
-    <row r="86" spans="2:7">
+    <row r="86" spans="2:9">
       <c r="B86" t="s">
         <v>19</v>
       </c>
       <c r="D86">
         <v>363</v>
       </c>
-      <c r="E86">
+      <c r="F86">
         <v>27</v>
       </c>
-      <c r="G86">
+      <c r="I86">
         <v>26.460160586800001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Switch to a statistically valid version of the chi-squared test
</commit_message>
<xml_diff>
--- a/InspectedTopWords.xlsx
+++ b/InspectedTopWords.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27220" yWindow="0" windowWidth="27640" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="51080" yWindow="-7060" windowWidth="21720" windowHeight="37940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="97">
   <si>
     <t>wife</t>
   </si>
@@ -292,6 +292,24 @@
   </si>
   <si>
     <t>% Other</t>
+  </si>
+  <si>
+    <t>Male Democrats</t>
+  </si>
+  <si>
+    <t>Female Democrats</t>
+  </si>
+  <si>
+    <t>district map</t>
+  </si>
+  <si>
+    <t>Female Rep</t>
+  </si>
+  <si>
+    <t>Male Rep</t>
+  </si>
+  <si>
+    <t>district</t>
   </si>
 </sst>
 </file>
@@ -355,8 +373,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -494,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="165">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -560,6 +612,23 @@
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -625,6 +694,23 @@
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -954,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:X86"/>
+  <dimension ref="A3:X105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H103" sqref="H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1321,14 +1407,14 @@
         <v>36</v>
       </c>
       <c r="E16">
-        <f t="shared" ref="E16:E26" si="2">D16/$B$14 * 100</f>
+        <f>D16/$B$14 * 100</f>
         <v>33.333333333333329</v>
       </c>
       <c r="F16">
         <v>69</v>
       </c>
       <c r="G16">
-        <f t="shared" ref="G16:G26" si="3">F16/$B$3 * 100</f>
+        <f>F16/$B$3 * 100</f>
         <v>15.898617511520738</v>
       </c>
       <c r="H16" t="b">
@@ -1359,38 +1445,35 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="1"/>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17">
-        <v>0.141961085509</v>
+      <c r="B17">
+        <v>2016</v>
       </c>
       <c r="D17">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
-        <v>30.555555555555557</v>
+        <f>D17/$B$14 * 100</f>
+        <v>5.5555555555555554</v>
       </c>
       <c r="F17">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="G17">
-        <f t="shared" si="3"/>
-        <v>16.359447004608295</v>
+        <f>F17/$B$3 * 100</f>
+        <v>0.69124423963133641</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>387.555454811</v>
+        <v>2234.9877297399998</v>
       </c>
       <c r="J17">
         <f>1/I17</f>
-        <v>2.5802759000971157E-3</v>
+        <v>4.4742974947622278E-4</v>
       </c>
       <c r="K17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="M17" t="s">
         <v>27</v>
@@ -1401,34 +1484,31 @@
     </row>
     <row r="18" spans="1:14">
       <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18">
-        <v>0.20579450418199999</v>
+        <v>30</v>
       </c>
       <c r="D18">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
-        <v>65.740740740740748</v>
+        <f>D18/$B$14 * 100</f>
+        <v>2.7777777777777777</v>
       </c>
       <c r="F18">
-        <v>196</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <f t="shared" si="3"/>
-        <v>45.161290322580641</v>
+        <f>F18/$B$3 * 100</f>
+        <v>0</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>156.3130572</v>
+        <v>1936.5487168300001</v>
       </c>
       <c r="J18">
         <f>1/I18</f>
-        <v>6.3974182190072344E-3</v>
+        <v>5.1638256828205836E-4</v>
       </c>
       <c r="K18" t="s">
         <v>41</v>
@@ -1438,96 +1518,102 @@
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="B19">
-        <v>2016</v>
+      <c r="B19" t="s">
+        <v>23</v>
       </c>
       <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <f>D19/$B$14 * 100</f>
+        <v>6.481481481481481</v>
+      </c>
+      <c r="F19">
         <v>6</v>
       </c>
-      <c r="E19">
-        <f t="shared" si="2"/>
-        <v>5.5555555555555554</v>
-      </c>
-      <c r="F19">
-        <v>3</v>
-      </c>
       <c r="G19">
-        <f t="shared" si="3"/>
-        <v>0.69124423963133641</v>
+        <f>F19/$B$3 * 100</f>
+        <v>1.3824884792626728</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>2234.9877297399998</v>
+        <v>454.44544024099997</v>
       </c>
       <c r="J19">
         <f>1/I19</f>
-        <v>4.4742974947622278E-4</v>
+        <v>2.2004841757674661E-3</v>
       </c>
       <c r="K19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="B20" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>0.141961085509</v>
       </c>
       <c r="D20">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
-        <v>6.481481481481481</v>
+        <f>D20/$B$14 * 100</f>
+        <v>30.555555555555557</v>
       </c>
       <c r="F20">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
-        <v>1.3824884792626728</v>
+        <f>F20/$B$3 * 100</f>
+        <v>16.359447004608295</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>454.44544024099997</v>
+        <v>387.555454811</v>
       </c>
       <c r="J20">
         <f>1/I20</f>
-        <v>2.2004841757674661E-3</v>
+        <v>2.5802759000971157E-3</v>
       </c>
       <c r="K20" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="B21" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>0.20579450418199999</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="E21">
-        <f t="shared" si="2"/>
-        <v>2.7777777777777777</v>
+        <f>D21/$B$14 * 100</f>
+        <v>65.740740740740748</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="G21">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>F21/$B$3 * 100</f>
+        <v>45.161290322580641</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>1936.5487168300001</v>
+        <v>156.3130572</v>
       </c>
       <c r="J21">
         <f>1/I21</f>
-        <v>5.1638256828205836E-4</v>
+        <v>6.3974182190072344E-3</v>
       </c>
       <c r="K21" t="s">
         <v>41</v>
@@ -1541,14 +1627,14 @@
         <v>6</v>
       </c>
       <c r="E22">
-        <f t="shared" si="2"/>
+        <f>D22/$B$14 * 100</f>
         <v>5.5555555555555554</v>
       </c>
       <c r="F22">
         <v>6</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
+        <f>F22/$B$3 * 100</f>
         <v>1.3824884792626728</v>
       </c>
       <c r="H22" t="b">
@@ -1567,87 +1653,78 @@
     </row>
     <row r="23" spans="1:14">
       <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23">
-        <v>0.15962621607800001</v>
+        <v>32</v>
       </c>
       <c r="D23">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="E23">
-        <f t="shared" si="2"/>
-        <v>63.888888888888886</v>
+        <f>D23/$B$14 * 100</f>
+        <v>6.481481481481481</v>
       </c>
       <c r="F23">
-        <v>208</v>
+        <v>9</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
-        <v>47.926267281105986</v>
+        <f>F23/$B$3 * 100</f>
+        <v>2.0737327188940093</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>26.418314666600001</v>
+        <v>58.6605817433</v>
       </c>
       <c r="J23">
         <f>1/I23</f>
-        <v>3.7852528165404679E-2</v>
+        <v>1.7047222688244417E-2</v>
       </c>
       <c r="K23" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="B24" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="D24">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E24">
-        <f t="shared" si="2"/>
-        <v>6.481481481481481</v>
+        <f>D24/$B$14 * 100</f>
+        <v>2.7777777777777777</v>
       </c>
       <c r="F24">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <f t="shared" si="3"/>
-        <v>2.0737327188940093</v>
-      </c>
-      <c r="H24" t="b">
-        <v>0</v>
+        <f>F24/$B$3 * 100</f>
+        <v>0.46082949308755761</v>
       </c>
       <c r="I24">
-        <v>58.6605817433</v>
+        <v>40.197394443599997</v>
       </c>
       <c r="J24">
         <f>1/I24</f>
-        <v>1.7047222688244417E-2</v>
-      </c>
-      <c r="K24" t="s">
-        <v>44</v>
+        <v>2.4877234304404385E-2</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="B25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D25">
         <v>3</v>
       </c>
       <c r="E25">
-        <f t="shared" si="2"/>
+        <f>D25/$B$14 * 100</f>
         <v>2.7777777777777777</v>
       </c>
       <c r="F25">
         <v>2</v>
       </c>
       <c r="G25">
-        <f t="shared" si="3"/>
+        <f>F25/$B$3 * 100</f>
         <v>0.46082949308755761</v>
       </c>
       <c r="I25">
@@ -1660,28 +1737,37 @@
     </row>
     <row r="26" spans="1:14">
       <c r="B26" t="s">
-        <v>88</v>
+        <v>18</v>
+      </c>
+      <c r="C26">
+        <v>0.15962621607800001</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="E26">
-        <f t="shared" si="2"/>
-        <v>2.7777777777777777</v>
+        <f>D26/$B$14 * 100</f>
+        <v>63.888888888888886</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>208</v>
       </c>
       <c r="G26">
-        <f t="shared" si="3"/>
-        <v>0.46082949308755761</v>
+        <f>F26/$B$3 * 100</f>
+        <v>47.926267281105986</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>40.197394443599997</v>
+        <v>26.418314666600001</v>
       </c>
       <c r="J26">
         <f>1/I26</f>
-        <v>2.4877234304404385E-2</v>
+        <v>3.7852528165404679E-2</v>
+      </c>
+      <c r="K26" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -1732,14 +1818,14 @@
         <v>13</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E40" si="4">D34/$B$32 * 100</f>
+        <f t="shared" ref="E34:E40" si="2">D34/$B$32 * 100</f>
         <v>5.6034482758620694</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34">
-        <f t="shared" ref="G34:G40" si="5">F34/$B$41 * 100</f>
+        <f t="shared" ref="G34:G40" si="3">F34/$B$41 * 100</f>
         <v>0</v>
       </c>
       <c r="H34" t="b">
@@ -1761,14 +1847,14 @@
         <v>12</v>
       </c>
       <c r="E35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>5.1724137931034484</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H35" t="b">
@@ -1790,14 +1876,14 @@
         <v>9</v>
       </c>
       <c r="E36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>3.8793103448275863</v>
       </c>
       <c r="F36">
         <v>0</v>
       </c>
       <c r="G36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H36" t="b">
@@ -1822,14 +1908,14 @@
         <v>14</v>
       </c>
       <c r="E37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>6.0344827586206895</v>
       </c>
       <c r="F37">
         <v>3</v>
       </c>
       <c r="G37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H37" t="b">
@@ -1851,14 +1937,14 @@
         <v>12</v>
       </c>
       <c r="E38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>5.1724137931034484</v>
       </c>
       <c r="F38">
         <v>4</v>
       </c>
       <c r="G38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.3333333333333335</v>
       </c>
       <c r="H38" t="b">
@@ -1880,14 +1966,14 @@
         <v>4</v>
       </c>
       <c r="E39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.7241379310344827</v>
       </c>
       <c r="F39">
         <v>0</v>
       </c>
       <c r="G39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H39" t="b">
@@ -1909,14 +1995,14 @@
         <v>4</v>
       </c>
       <c r="E40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.7241379310344827</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
       <c r="G40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H40" t="b">
@@ -1963,7 +2049,7 @@
         <v>12539.9444358</v>
       </c>
       <c r="J42">
-        <f t="shared" ref="J35:J49" si="6">1/I42</f>
+        <f t="shared" ref="J35:J49" si="4">1/I42</f>
         <v>7.9745169934335825E-5</v>
       </c>
       <c r="K42" t="s">
@@ -1978,14 +2064,14 @@
         <v>13</v>
       </c>
       <c r="E43">
-        <f t="shared" ref="E43:E49" si="7">D43/$B$41 * 100</f>
+        <f t="shared" ref="E43:E49" si="5">D43/$B$41 * 100</f>
         <v>4.3333333333333339</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
-        <f t="shared" ref="G43:G49" si="8">F43/$B$32 * 100</f>
+        <f t="shared" ref="G43:G49" si="6">F43/$B$32 * 100</f>
         <v>0</v>
       </c>
       <c r="H43" t="b">
@@ -1995,7 +2081,7 @@
         <v>743.23048311299999</v>
       </c>
       <c r="J43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.345477644850529E-3</v>
       </c>
     </row>
@@ -2007,14 +2093,14 @@
         <v>40</v>
       </c>
       <c r="E44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>13.333333333333334</v>
       </c>
       <c r="F44">
         <v>13</v>
       </c>
       <c r="G44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>5.6034482758620694</v>
       </c>
       <c r="H44" t="b">
@@ -2024,7 +2110,7 @@
         <v>249.50530092899999</v>
       </c>
       <c r="J44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4.0079308787293591E-3</v>
       </c>
     </row>
@@ -2036,14 +2122,14 @@
         <v>20</v>
       </c>
       <c r="E45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>6.666666666666667</v>
       </c>
       <c r="F45">
         <v>5</v>
       </c>
       <c r="G45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.1551724137931036</v>
       </c>
       <c r="H45" t="b">
@@ -2053,7 +2139,7 @@
         <v>66.643996215300007</v>
       </c>
       <c r="J45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.5005102586726661E-2</v>
       </c>
     </row>
@@ -2065,14 +2151,14 @@
         <v>7</v>
       </c>
       <c r="E46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>2.3333333333333335</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
       <c r="G46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H46" t="b">
@@ -2082,7 +2168,7 @@
         <v>53.645178920799999</v>
       </c>
       <c r="J46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.8641004096125163E-2</v>
       </c>
     </row>
@@ -2094,14 +2180,14 @@
         <v>38</v>
       </c>
       <c r="E47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>12.666666666666668</v>
       </c>
       <c r="F47">
         <v>15</v>
       </c>
       <c r="G47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>6.4655172413793105</v>
       </c>
       <c r="H47" t="b">
@@ -2111,7 +2197,7 @@
         <v>49.728274775199999</v>
       </c>
       <c r="J47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.0109283994278245E-2</v>
       </c>
     </row>
@@ -2123,14 +2209,14 @@
         <v>5</v>
       </c>
       <c r="E48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
       <c r="G48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H48" t="b">
@@ -2140,7 +2226,7 @@
         <v>21.3792568876</v>
       </c>
       <c r="J48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4.6774310503748209E-2</v>
       </c>
     </row>
@@ -2152,14 +2238,14 @@
         <v>5</v>
       </c>
       <c r="E49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="F49">
         <v>0</v>
       </c>
       <c r="G49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H49" t="b">
@@ -2169,7 +2255,7 @@
         <v>21.3792568876</v>
       </c>
       <c r="J49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4.6774310503748209E-2</v>
       </c>
     </row>
@@ -2558,7 +2644,7 @@
         <v>41.3462003307</v>
       </c>
     </row>
-    <row r="81" spans="2:9">
+    <row r="81" spans="1:10">
       <c r="B81">
         <v>2016</v>
       </c>
@@ -2572,7 +2658,7 @@
         <v>37.610324992499997</v>
       </c>
     </row>
-    <row r="82" spans="2:9">
+    <row r="82" spans="1:10">
       <c r="B82" t="s">
         <v>24</v>
       </c>
@@ -2586,7 +2672,7 @@
         <v>27.355121940899998</v>
       </c>
     </row>
-    <row r="83" spans="2:9">
+    <row r="83" spans="1:10">
       <c r="B83" t="s">
         <v>74</v>
       </c>
@@ -2600,7 +2686,7 @@
         <v>27.355121940899998</v>
       </c>
     </row>
-    <row r="84" spans="2:9">
+    <row r="84" spans="1:10">
       <c r="B84" t="s">
         <v>75</v>
       </c>
@@ -2614,7 +2700,7 @@
         <v>27.355121940899998</v>
       </c>
     </row>
-    <row r="85" spans="2:9">
+    <row r="85" spans="1:10">
       <c r="B85" t="s">
         <v>76</v>
       </c>
@@ -2628,7 +2714,7 @@
         <v>27.355121940899998</v>
       </c>
     </row>
-    <row r="86" spans="2:9">
+    <row r="86" spans="1:10">
       <c r="B86" t="s">
         <v>19</v>
       </c>
@@ -2642,9 +2728,211 @@
         <v>26.460160586800001</v>
       </c>
     </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="B92" t="s">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>10</v>
+      </c>
+      <c r="E92">
+        <f>D92/$B$91*100</f>
+        <v>6.2893081761006293</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>38.741330766300003</v>
+      </c>
+      <c r="J92">
+        <f>1/I92</f>
+        <v>2.5812226379943355E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B95">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="B96" t="s">
+        <v>17</v>
+      </c>
+      <c r="D96">
+        <v>24</v>
+      </c>
+      <c r="E96">
+        <f>D96/$B$95*100</f>
+        <v>30.37974683544304</v>
+      </c>
+      <c r="F96">
+        <v>21</v>
+      </c>
+      <c r="G96">
+        <f>F96/$B$91*100</f>
+        <v>13.20754716981132</v>
+      </c>
+      <c r="I96">
+        <v>242.85920955700001</v>
+      </c>
+      <c r="J96">
+        <f>1/I96</f>
+        <v>4.1176120181898894E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="B97" t="s">
+        <v>93</v>
+      </c>
+      <c r="D97">
+        <v>9</v>
+      </c>
+      <c r="E97">
+        <f t="shared" ref="E97:E99" si="7">D97/$B$95*100</f>
+        <v>11.39240506329114</v>
+      </c>
+      <c r="F97">
+        <v>5</v>
+      </c>
+      <c r="G97">
+        <f t="shared" ref="G97:G99" si="8">F97/$B$91*100</f>
+        <v>3.1446540880503147</v>
+      </c>
+      <c r="I97">
+        <v>74.114175263800007</v>
+      </c>
+      <c r="J97">
+        <f t="shared" ref="J97:J99" si="9">1/I97</f>
+        <v>1.3492695512574036E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="B98" t="s">
+        <v>16</v>
+      </c>
+      <c r="D98">
+        <v>56</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="7"/>
+        <v>70.886075949367083</v>
+      </c>
+      <c r="F98">
+        <v>73</v>
+      </c>
+      <c r="G98">
+        <f t="shared" si="8"/>
+        <v>45.911949685534594</v>
+      </c>
+      <c r="I98">
+        <v>72.859334163900002</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="9"/>
+        <v>1.3725077390227857E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="B99" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99">
+        <v>34</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="7"/>
+        <v>43.037974683544306</v>
+      </c>
+      <c r="F99">
+        <v>42</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="8"/>
+        <v>26.415094339622641</v>
+      </c>
+      <c r="I99">
+        <v>30.679398791899999</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="9"/>
+        <v>3.2595162857755246E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B102">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B103">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="B104" t="s">
+        <v>17</v>
+      </c>
+      <c r="D104">
+        <v>12</v>
+      </c>
+      <c r="E104">
+        <f>D104/$B$103*100</f>
+        <v>41.379310344827587</v>
+      </c>
+      <c r="F104">
+        <v>48</v>
+      </c>
+      <c r="G104">
+        <f>F104/$B$102 * 100</f>
+        <v>17.647058823529413</v>
+      </c>
+      <c r="I104">
+        <v>30.9332029015</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="B105" t="s">
+        <v>96</v>
+      </c>
+      <c r="D105">
+        <v>9</v>
+      </c>
+      <c r="E105">
+        <f>D105/$B$103*100</f>
+        <v>31.03448275862069</v>
+      </c>
+      <c r="F105">
+        <v>38</v>
+      </c>
+      <c r="G105">
+        <f>F105/$B$102 * 100</f>
+        <v>13.970588235294118</v>
+      </c>
+      <c r="I105">
+        <v>153.69888408700001</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="B5:H14">
-    <sortCondition ref="H5:H14"/>
+  <sortState ref="B15:K26">
+    <sortCondition ref="J15:J26"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Cleaned up code, removed clutter from repository
</commit_message>
<xml_diff>
--- a/InspectedTopWords.xlsx
+++ b/InspectedTopWords.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="51080" yWindow="-7060" windowWidth="21720" windowHeight="37940" tabRatio="500"/>
+    <workbookView xWindow="51120" yWindow="-7060" windowWidth="21720" windowHeight="37940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
   <si>
     <t>wife</t>
   </si>
@@ -42,9 +42,6 @@
     <t>congress</t>
   </si>
   <si>
-    <t>committee assignments</t>
-  </si>
-  <si>
     <t>obituary</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>donald trump</t>
   </si>
   <si>
-    <t>ballotpedia</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -111,18 +105,9 @@
     <t>chi squared P value</t>
   </si>
   <si>
-    <t>district office</t>
-  </si>
-  <si>
     <t>hillary clinton</t>
   </si>
   <si>
-    <t>cuba</t>
-  </si>
-  <si>
-    <t>married</t>
-  </si>
-  <si>
     <t>pronunciation</t>
   </si>
   <si>
@@ -135,12 +120,6 @@
     <t>?????</t>
   </si>
   <si>
-    <t>Republicans skew male</t>
-  </si>
-  <si>
-    <t>More "generic" male names? Same with name collision?</t>
-  </si>
-  <si>
     <t>More interest in life stories of underrepresented groups?</t>
   </si>
   <si>
@@ -153,9 +132,6 @@
     <t>Dems skew female?</t>
   </si>
   <si>
-    <t>Dems skew female, Cuba an Obama initiative?</t>
-  </si>
-  <si>
     <t>Democrat</t>
   </si>
   <si>
@@ -168,9 +144,6 @@
     <t>tpp</t>
   </si>
   <si>
-    <t>iran deal</t>
-  </si>
-  <si>
     <t>israel</t>
   </si>
   <si>
@@ -186,18 +159,9 @@
     <t>Harry Reid had some comments on Trump</t>
   </si>
   <si>
-    <t>phone number</t>
-  </si>
-  <si>
     <t>voting record</t>
   </si>
   <si>
-    <t>rubio</t>
-  </si>
-  <si>
-    <t>photography</t>
-  </si>
-  <si>
     <t>This seems like the biggest story</t>
   </si>
   <si>
@@ -255,18 +219,9 @@
     <t>Rejected for name collsion:</t>
   </si>
   <si>
-    <t>Most popular female name %</t>
-  </si>
-  <si>
-    <t>Most popular male name %</t>
-  </si>
-  <si>
     <t>http://names.mongabay.com/female_names.htm</t>
   </si>
   <si>
-    <t>None of the rest of these are statistically significant</t>
-  </si>
-  <si>
     <t>artist</t>
   </si>
   <si>
@@ -282,12 +237,6 @@
     <t>campaign manager</t>
   </si>
   <si>
-    <t>vice president</t>
-  </si>
-  <si>
-    <t>poll</t>
-  </si>
-  <si>
     <t>% Matching</t>
   </si>
   <si>
@@ -310,13 +259,23 @@
   </si>
   <si>
     <t>district</t>
+  </si>
+  <si>
+    <t>twitter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -373,180 +332,326 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="165">
+  <cellStyleXfs count="308">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="165" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="165">
+  <cellStyles count="308">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -629,6 +734,77 @@
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="303" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="305" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="307" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -711,7 +887,79 @@
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="286" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="290" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="292" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="294" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="296" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="298" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="300" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="302" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="304" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="306" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="165" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1042,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:X105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H103" sqref="H103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1063,7 +1311,7 @@
         <v>434</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -1077,224 +1325,161 @@
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:24">
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>7.1428571428599999E-2</v>
+      <c r="C5" s="5">
+        <f>E5-G5</f>
+        <v>7.8341013824884786E-2</v>
       </c>
       <c r="D5">
-        <v>31</v>
-      </c>
-      <c r="E5">
-        <f>D5/$B$3 * 100</f>
-        <v>7.1428571428571423</v>
+        <v>34</v>
+      </c>
+      <c r="E5" s="5">
+        <f>D5/$B$3</f>
+        <v>7.8341013824884786E-2</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5">
-        <f>F5/$B$14 * 100</f>
+      <c r="G5" s="5">
+        <f>F5/$B$14</f>
         <v>0</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>182.529940977</v>
+        <v>185.54240429500001</v>
       </c>
       <c r="J5">
         <f>1/I5</f>
-        <v>5.4785532425390242E-3</v>
+        <v>5.3896035453440978E-3</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="N5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6">
-        <v>5.0605905444600002E-2</v>
+      <c r="C6" s="5">
+        <f t="shared" ref="C6:C7" si="0">E6-G6</f>
+        <v>5.5299539170506916E-2</v>
       </c>
       <c r="D6">
-        <v>30</v>
-      </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E9" si="0">D6/$B$3 * 100</f>
-        <v>6.9124423963133648</v>
+        <v>24</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" ref="E6:E7" si="1">D6/$B$3</f>
+        <v>5.5299539170506916E-2</v>
       </c>
       <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <f t="shared" ref="G6:G9" si="1">F6/$B$14 * 100</f>
-        <v>1.8518518518518516</v>
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" ref="G6:G7" si="2">F6/$B$14</f>
+        <v>0</v>
       </c>
       <c r="H6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>18.949877262800001</v>
+        <v>39.695650727100002</v>
       </c>
       <c r="J6">
         <f>1/I6</f>
-        <v>5.277079033979145E-2</v>
+        <v>2.5191676712262724E-2</v>
       </c>
       <c r="K6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="N6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:24">
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7">
-        <v>1.84331797235E-2</v>
+        <v>6</v>
+      </c>
+      <c r="C7" s="5">
+        <f t="shared" si="0"/>
+        <v>9.1781874039938552E-2</v>
       </c>
       <c r="D7">
-        <v>8</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1.8433179723502304</v>
+        <v>76</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.17511520737327188</v>
       </c>
       <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="2"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>6.3187563209900004</v>
+        <v>35.899836518299999</v>
       </c>
       <c r="J7">
         <f>1/I7</f>
-        <v>0.15825899104197827</v>
-      </c>
-      <c r="K7" t="s">
-        <v>38</v>
+        <v>2.785528005093417E-2</v>
       </c>
       <c r="N7" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="V7" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:24">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>6.6393582522599998E-2</v>
-      </c>
-      <c r="D8">
-        <v>69</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>15.898617511520738</v>
-      </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="1"/>
-        <v>9.2592592592592595</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>9.4490591251199998</v>
-      </c>
-      <c r="J8">
-        <f>1/I8</f>
-        <v>0.1058306426871152</v>
-      </c>
-      <c r="K8" t="s">
-        <v>39</v>
-      </c>
+      <c r="E8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:24">
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9">
-        <v>1.6129032258100001E-2</v>
-      </c>
-      <c r="D9">
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>1.6129032258064515</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>5.3506330028400004</v>
-      </c>
-      <c r="J9">
-        <f>1/I9</f>
-        <v>0.18689377489901132</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="V9" s="1"/>
+      <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:24">
+      <c r="E10" s="4"/>
+      <c r="G10" s="4"/>
       <c r="V10">
         <v>2.629</v>
       </c>
@@ -1303,8 +1488,10 @@
       </c>
     </row>
     <row r="11" spans="1:24">
+      <c r="E11" s="4"/>
+      <c r="G11" s="4"/>
       <c r="N11" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="V11">
         <v>1.073</v>
@@ -1314,8 +1501,10 @@
       </c>
     </row>
     <row r="12" spans="1:24">
+      <c r="E12" s="4"/>
+      <c r="G12" s="4"/>
       <c r="N12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="V12">
         <v>1.0349999999999999</v>
@@ -1325,8 +1514,10 @@
       </c>
     </row>
     <row r="13" spans="1:24">
+      <c r="E13" s="4"/>
+      <c r="G13" s="4"/>
       <c r="N13" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="V13">
         <v>0.98</v>
@@ -1337,13 +1528,15 @@
     </row>
     <row r="14" spans="1:24">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>108</v>
       </c>
+      <c r="E14" s="4"/>
+      <c r="G14" s="4"/>
       <c r="N14" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="V14">
         <v>0.93700000000000006</v>
@@ -1354,40 +1547,41 @@
     </row>
     <row r="15" spans="1:24">
       <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15">
-        <v>7.4074074074099994E-2</v>
+        <v>21</v>
+      </c>
+      <c r="C15" s="5">
+        <f>E15-G15</f>
+        <v>7.407407407407407E-2</v>
       </c>
       <c r="D15">
         <v>8</v>
       </c>
-      <c r="E15">
-        <f>D15/$B$14 * 100</f>
-        <v>7.4074074074074066</v>
+      <c r="E15" s="6">
+        <f>D15/$B$14</f>
+        <v>7.407407407407407E-2</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
-      <c r="G15">
-        <f>F15/$B$3 * 100</f>
+      <c r="G15" s="5">
+        <f>F15/$B$3</f>
         <v>0</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>70002132.604000002</v>
+        <v>7187360.1435599998</v>
       </c>
       <c r="J15">
         <f>1/I15</f>
-        <v>1.4285279073667233E-8</v>
+        <v>1.3913314207526075E-7</v>
       </c>
       <c r="K15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="N15" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="V15">
         <v>0.93200000000000005</v>
@@ -1398,873 +1592,746 @@
     </row>
     <row r="16" spans="1:24">
       <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16">
-        <v>0.17434715821800001</v>
+        <v>15</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" ref="C16:C24" si="3">E16-G16</f>
+        <v>0.26830517153097799</v>
       </c>
       <c r="D16">
-        <v>36</v>
-      </c>
-      <c r="E16">
-        <f>D16/$B$14 * 100</f>
-        <v>33.333333333333329</v>
+        <v>78</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" ref="E16:E24" si="4">D16/$B$14</f>
+        <v>0.72222222222222221</v>
       </c>
       <c r="F16">
-        <v>69</v>
-      </c>
-      <c r="G16">
-        <f>F16/$B$3 * 100</f>
-        <v>15.898617511520738</v>
+        <v>197</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" ref="G16:G24" si="5">F16/$B$3</f>
+        <v>0.45391705069124422</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>4349.1771987299999</v>
+        <v>957949.46424600005</v>
       </c>
       <c r="J16">
         <f>1/I16</f>
-        <v>2.2992854839117829E-4</v>
+        <v>1.0438964030186058E-6</v>
       </c>
       <c r="K16" t="s">
-        <v>40</v>
-      </c>
-      <c r="N16" t="s">
-        <v>86</v>
-      </c>
-      <c r="V16" s="1">
-        <f>SUM(V10:V15)</f>
-        <v>7.5860000000000012</v>
-      </c>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1">
-        <f>SUM(X10:X15)</f>
-        <v>17.175000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="1"/>
-      <c r="B17">
-        <v>2016</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" si="3"/>
+        <v>0.26830517153097799</v>
       </c>
       <c r="D17">
-        <v>6</v>
-      </c>
-      <c r="E17">
-        <f>D17/$B$14 * 100</f>
-        <v>5.5555555555555554</v>
+        <v>78</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="4"/>
+        <v>0.72222222222222221</v>
       </c>
       <c r="F17">
-        <v>3</v>
-      </c>
-      <c r="G17">
-        <f>F17/$B$3 * 100</f>
-        <v>0.69124423963133641</v>
+        <v>197</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="5"/>
+        <v>0.45391705069124422</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>2234.9877297399998</v>
+        <v>5418.2530677300001</v>
       </c>
       <c r="J17">
         <f>1/I17</f>
-        <v>4.4742974947622278E-4</v>
-      </c>
-      <c r="K17" t="s">
-        <v>42</v>
-      </c>
-      <c r="M17" t="s">
-        <v>27</v>
-      </c>
-      <c r="N17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>1.8456133139217769E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
       <c r="B18" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" si="3"/>
+        <v>0.15117767537122379</v>
       </c>
       <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="E18">
-        <f>D18/$B$14 * 100</f>
-        <v>2.7777777777777777</v>
+        <v>33</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.30555555555555558</v>
       </c>
       <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <f>F18/$B$3 * 100</f>
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="5"/>
+        <v>0.15437788018433179</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>1936.5487168300001</v>
+        <v>2037.7433038900001</v>
       </c>
       <c r="J18">
         <f>1/I18</f>
-        <v>5.1638256828205836E-4</v>
+        <v>4.9073894542606296E-4</v>
       </c>
       <c r="K18" t="s">
-        <v>41</v>
-      </c>
-      <c r="N18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="B19" t="s">
-        <v>23</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="A19" s="1"/>
+      <c r="B19">
+        <v>2016</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" si="3"/>
+        <v>4.8643113159242191E-2</v>
       </c>
       <c r="D19">
-        <v>7</v>
-      </c>
-      <c r="E19">
-        <f>D19/$B$14 * 100</f>
-        <v>6.481481481481481</v>
+        <v>6</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="4"/>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="F19">
-        <v>6</v>
-      </c>
-      <c r="G19">
-        <f>F19/$B$3 * 100</f>
-        <v>1.3824884792626728</v>
+        <v>3</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="5"/>
+        <v>6.9124423963133645E-3</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>454.44544024099997</v>
+        <v>551.37124177099997</v>
       </c>
       <c r="J19">
         <f>1/I19</f>
-        <v>2.2004841757674661E-3</v>
+        <v>1.8136600610289505E-3</v>
       </c>
       <c r="K19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>35</v>
+      </c>
+      <c r="M19" t="s">
+        <v>25</v>
+      </c>
+      <c r="N19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
       <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20">
-        <v>0.141961085509</v>
+        <v>80</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" si="3"/>
+        <v>0.14904420549581832</v>
       </c>
       <c r="D20">
-        <v>33</v>
-      </c>
-      <c r="E20">
-        <f>D20/$B$14 * 100</f>
-        <v>30.555555555555557</v>
+        <v>91</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" si="4"/>
+        <v>0.84259259259259256</v>
       </c>
       <c r="F20">
-        <v>71</v>
-      </c>
-      <c r="G20">
-        <f>F20/$B$3 * 100</f>
-        <v>16.359447004608295</v>
+        <v>301</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="5"/>
+        <v>0.69354838709677424</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>387.555454811</v>
+        <v>344.477582713</v>
       </c>
       <c r="J20">
         <f>1/I20</f>
-        <v>2.5802759000971157E-3</v>
-      </c>
-      <c r="K20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+        <v>2.9029465201314583E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
       <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="C21">
-        <v>0.20579450418199999</v>
+      <c r="C21" s="5">
+        <f t="shared" si="3"/>
+        <v>0.12813620071684589</v>
       </c>
       <c r="D21">
-        <v>71</v>
-      </c>
-      <c r="E21">
-        <f>D21/$B$14 * 100</f>
-        <v>65.740740740740748</v>
+        <v>33</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="4"/>
+        <v>0.30555555555555558</v>
       </c>
       <c r="F21">
-        <v>196</v>
-      </c>
-      <c r="G21">
-        <f>F21/$B$3 * 100</f>
-        <v>45.161290322580641</v>
+        <v>77</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="5"/>
+        <v>0.17741935483870969</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>156.3130572</v>
+        <v>214.18415042399999</v>
       </c>
       <c r="J21">
         <f>1/I21</f>
-        <v>6.3974182190072344E-3</v>
+        <v>4.6688795507062271E-3</v>
       </c>
       <c r="K21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>33</v>
+      </c>
+      <c r="N21" t="s">
+        <v>71</v>
+      </c>
+      <c r="V21" s="1">
+        <f>SUM(V14:V19)</f>
+        <v>1.8690000000000002</v>
+      </c>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1">
+        <f>SUM(X14:X19)</f>
+        <v>4.8140000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
       <c r="B22" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" si="3"/>
+        <v>6.0291858678955451E-2</v>
       </c>
       <c r="D22">
-        <v>6</v>
-      </c>
-      <c r="E22">
-        <f>D22/$B$14 * 100</f>
-        <v>5.5555555555555554</v>
+        <v>9</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="4"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F22">
-        <v>6</v>
-      </c>
-      <c r="G22">
-        <f>F22/$B$3 * 100</f>
-        <v>1.3824884792626728</v>
+        <v>10</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="5"/>
+        <v>2.3041474654377881E-2</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
       </c>
       <c r="I22">
-        <v>109.828857324</v>
+        <v>170.99157950700001</v>
       </c>
       <c r="J22">
         <f>1/I22</f>
-        <v>9.1050751538819686E-3</v>
+        <v>5.8482411992636296E-3</v>
       </c>
       <c r="K22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
       <c r="B23" t="s">
-        <v>32</v>
+        <v>17</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" si="3"/>
+        <v>0.15962621607782895</v>
       </c>
       <c r="D23">
-        <v>7</v>
-      </c>
-      <c r="E23">
-        <f>D23/$B$14 * 100</f>
-        <v>6.481481481481481</v>
+        <v>69</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="4"/>
+        <v>0.63888888888888884</v>
       </c>
       <c r="F23">
-        <v>9</v>
-      </c>
-      <c r="G23">
-        <f>F23/$B$3 * 100</f>
-        <v>2.0737327188940093</v>
+        <v>208</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" si="5"/>
+        <v>0.47926267281105989</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>58.6605817433</v>
+        <v>122.592017234</v>
       </c>
       <c r="J23">
         <f>1/I23</f>
-        <v>1.7047222688244417E-2</v>
+        <v>8.1571379814334051E-3</v>
       </c>
       <c r="K23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
       <c r="B24" t="s">
-        <v>87</v>
+        <v>22</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" si="3"/>
+        <v>4.8685782556750296E-2</v>
       </c>
       <c r="D24">
-        <v>3</v>
-      </c>
-      <c r="E24">
-        <f>D24/$B$14 * 100</f>
-        <v>2.7777777777777777</v>
+        <v>7</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="4"/>
+        <v>6.4814814814814811E-2</v>
       </c>
       <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="G24">
-        <f>F24/$B$3 * 100</f>
-        <v>0.46082949308755761</v>
+        <v>7</v>
+      </c>
+      <c r="G24" s="5">
+        <f t="shared" si="5"/>
+        <v>1.6129032258064516E-2</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>40.197394443599997</v>
+        <v>84.060451375300005</v>
       </c>
       <c r="J24">
         <f>1/I24</f>
-        <v>2.4877234304404385E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="B25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-      <c r="E25">
-        <f>D25/$B$14 * 100</f>
-        <v>2.7777777777777777</v>
-      </c>
-      <c r="F25">
-        <v>2</v>
-      </c>
-      <c r="G25">
-        <f>F25/$B$3 * 100</f>
-        <v>0.46082949308755761</v>
-      </c>
-      <c r="I25">
-        <v>40.197394443599997</v>
-      </c>
-      <c r="J25">
-        <f>1/I25</f>
-        <v>2.4877234304404385E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26">
-        <v>0.15962621607800001</v>
-      </c>
-      <c r="D26">
-        <v>69</v>
-      </c>
-      <c r="E26">
-        <f>D26/$B$14 * 100</f>
-        <v>63.888888888888886</v>
-      </c>
-      <c r="F26">
-        <v>208</v>
-      </c>
-      <c r="G26">
-        <f>F26/$B$3 * 100</f>
-        <v>47.926267281105986</v>
-      </c>
-      <c r="H26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>26.418314666600001</v>
-      </c>
-      <c r="J26">
-        <f>1/I26</f>
-        <v>3.7852528165404679E-2</v>
-      </c>
-      <c r="K26" t="s">
+        <v>1.1896200694133271E-2</v>
+      </c>
+      <c r="K24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24">
+      <c r="E25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:24">
+      <c r="E26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:24">
+      <c r="E27" s="4"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:24">
+      <c r="E28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:24">
+      <c r="E29" s="4"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:24">
+      <c r="E30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:24">
+      <c r="E31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:24">
+      <c r="A32" s="1" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="B32">
         <v>232</v>
       </c>
+      <c r="E32" s="4"/>
+      <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:11">
       <c r="B33" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="C33" s="5">
+        <f>E33-G33</f>
+        <v>8.1896551724137928E-2</v>
       </c>
       <c r="D33">
-        <v>66</v>
-      </c>
-      <c r="E33">
-        <f>D33/$B$32 * 100</f>
-        <v>28.448275862068968</v>
+        <v>19</v>
+      </c>
+      <c r="E33" s="5">
+        <f>D33/$B$32</f>
+        <v>8.1896551724137928E-2</v>
       </c>
       <c r="F33">
-        <v>37</v>
-      </c>
-      <c r="G33">
-        <f>F33/$B$41 * 100</f>
-        <v>12.333333333333334</v>
+        <v>0</v>
+      </c>
+      <c r="G33" s="5">
+        <f>F33/$B$41</f>
+        <v>0</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
       </c>
       <c r="I33">
-        <v>21416.988187700001</v>
+        <v>505290.60101599997</v>
       </c>
       <c r="J33">
         <f>1/I33</f>
-        <v>4.6691906034402652E-5</v>
-      </c>
-      <c r="K33" t="s">
-        <v>59</v>
+        <v>1.9790591750356644E-6</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="B34" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="C34" s="5">
+        <f t="shared" ref="C34:C37" si="6">E34-G34</f>
+        <v>6.0344827586206899E-2</v>
       </c>
       <c r="D34">
-        <v>13</v>
-      </c>
-      <c r="E34">
-        <f t="shared" ref="E34:E40" si="2">D34/$B$32 * 100</f>
-        <v>5.6034482758620694</v>
+        <v>14</v>
+      </c>
+      <c r="E34" s="5">
+        <f t="shared" ref="E34:E37" si="7">D34/$B$32</f>
+        <v>6.0344827586206899E-2</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
-      <c r="G34">
-        <f t="shared" ref="G34:G40" si="3">F34/$B$41 * 100</f>
+      <c r="G34" s="5">
+        <f t="shared" ref="G34:G37" si="8">F34/$B$41</f>
         <v>0</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
       </c>
       <c r="I34">
-        <v>19926.9822914</v>
+        <v>15192.3103001</v>
       </c>
       <c r="J34">
         <f>1/I34</f>
-        <v>5.0183213161762862E-5</v>
+        <v>6.5822773511505859E-5</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="B35" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="C35" s="5">
+        <f t="shared" si="6"/>
+        <v>0.12097701149425286</v>
       </c>
       <c r="D35">
-        <v>12</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="2"/>
-        <v>5.1724137931034484</v>
+        <v>59</v>
+      </c>
+      <c r="E35" s="5">
+        <f t="shared" si="7"/>
+        <v>0.25431034482758619</v>
       </c>
       <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="G35" s="5">
+        <f t="shared" si="8"/>
+        <v>0.13333333333333333</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
       </c>
       <c r="I35">
-        <v>10212.8422538</v>
+        <v>1080.1189136099999</v>
       </c>
       <c r="J35">
         <f>1/I35</f>
-        <v>9.7915935167599351E-5</v>
+        <v>9.2582398789571737E-4</v>
+      </c>
+      <c r="K35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="B36" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="C36" s="5">
+        <f t="shared" si="6"/>
+        <v>4.172413793103448E-2</v>
       </c>
       <c r="D36">
-        <v>9</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="2"/>
-        <v>3.8793103448275863</v>
+        <v>12</v>
+      </c>
+      <c r="E36" s="5">
+        <f t="shared" si="7"/>
+        <v>5.1724137931034482E-2</v>
       </c>
       <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="G36" s="5">
+        <f t="shared" si="8"/>
+        <v>0.01</v>
       </c>
       <c r="H36" t="b">
         <v>0</v>
       </c>
       <c r="I36">
-        <v>1348.7061188800001</v>
+        <v>98.812109710499996</v>
       </c>
       <c r="J36">
         <f>1/I36</f>
-        <v>7.4145137031811305E-4</v>
-      </c>
-      <c r="K36" t="s">
-        <v>53</v>
+        <v>1.0120217075921189E-2</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="B37" t="s">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="C37" s="5">
+        <f t="shared" si="6"/>
+        <v>3.2126436781609195E-2</v>
       </c>
       <c r="D37">
-        <v>14</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="2"/>
-        <v>6.0344827586206895</v>
+        <v>9</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" si="7"/>
+        <v>3.8793103448275863E-2</v>
       </c>
       <c r="F37">
-        <v>3</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" si="8"/>
+        <v>6.6666666666666671E-3</v>
       </c>
       <c r="H37" t="b">
         <v>0</v>
       </c>
       <c r="I37">
-        <v>659.51471604400001</v>
+        <v>39.323722149600002</v>
       </c>
       <c r="J37">
         <f>1/I37</f>
-        <v>1.5162663935663935E-3</v>
+        <v>2.5429942674187366E-2</v>
+      </c>
+      <c r="K37" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:11">
-      <c r="B38" t="s">
-        <v>32</v>
-      </c>
-      <c r="D38">
-        <v>12</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="2"/>
-        <v>5.1724137931034484</v>
-      </c>
-      <c r="F38">
-        <v>4</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="3"/>
-        <v>1.3333333333333335</v>
-      </c>
-      <c r="H38" t="b">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>77.094611647700006</v>
-      </c>
-      <c r="J38">
-        <f>1/I38</f>
-        <v>1.2971075132587861E-2</v>
-      </c>
+      <c r="E38" s="4"/>
+      <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="B39" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39">
-        <v>4</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="2"/>
-        <v>1.7241379310344827</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H39" t="b">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>40.8148861588</v>
-      </c>
-      <c r="J39">
-        <f>1/I39</f>
-        <v>2.4500864613691747E-2</v>
-      </c>
+      <c r="E39" s="4"/>
+      <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="B40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40">
-        <v>4</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="2"/>
-        <v>1.7241379310344827</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H40" t="b">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>40.8148861588</v>
-      </c>
-      <c r="J40">
-        <f>1/I40</f>
-        <v>2.4500864613691747E-2</v>
-      </c>
+      <c r="E40" s="4"/>
+      <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>300</v>
       </c>
+      <c r="E41" s="4"/>
+      <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:11">
       <c r="B42" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="C42" s="5">
+        <f t="shared" ref="C6:C46" si="9">E42-G42</f>
+        <v>9.2356321839080463E-2</v>
       </c>
       <c r="D42">
-        <v>23</v>
-      </c>
-      <c r="E42">
-        <f>D42/$B$41 * 100</f>
-        <v>7.6666666666666661</v>
+        <v>29</v>
+      </c>
+      <c r="E42" s="6">
+        <f>D42/$B$41</f>
+        <v>9.6666666666666665E-2</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
-      <c r="G42">
-        <f>F42/$B$32 * 100</f>
-        <v>0.43103448275862066</v>
+      <c r="G42" s="5">
+        <f>F42/$B$32</f>
+        <v>4.3103448275862068E-3</v>
       </c>
       <c r="H42" t="b">
         <v>0</v>
       </c>
       <c r="I42">
-        <v>12539.9444358</v>
+        <v>113440.790874</v>
       </c>
       <c r="J42">
-        <f t="shared" ref="J35:J49" si="4">1/I42</f>
-        <v>7.9745169934335825E-5</v>
+        <f t="shared" ref="J42:J45" si="10">1/I42</f>
+        <v>8.8151712650761713E-6</v>
       </c>
       <c r="K42" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="B43" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="C43" s="5">
+        <f t="shared" si="9"/>
+        <v>0.05</v>
       </c>
       <c r="D43">
-        <v>13</v>
-      </c>
-      <c r="E43">
-        <f t="shared" ref="E43:E49" si="5">D43/$B$41 * 100</f>
-        <v>4.3333333333333339</v>
+        <v>15</v>
+      </c>
+      <c r="E43" s="6">
+        <f t="shared" ref="E43:E46" si="11">D43/$B$41</f>
+        <v>0.05</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
-      <c r="G43">
-        <f t="shared" ref="G43:G49" si="6">F43/$B$32 * 100</f>
+      <c r="G43" s="5">
+        <f t="shared" ref="G43:G46" si="12">F43/$B$32</f>
         <v>0</v>
       </c>
       <c r="H43" t="b">
         <v>0</v>
       </c>
       <c r="I43">
-        <v>743.23048311299999</v>
+        <v>805.481209154</v>
       </c>
       <c r="J43">
-        <f t="shared" si="4"/>
-        <v>1.345477644850529E-3</v>
+        <f t="shared" si="10"/>
+        <v>1.2414938904041024E-3</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="B44" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C44" s="5">
+        <f t="shared" si="9"/>
+        <v>5.6321839080459769E-2</v>
       </c>
       <c r="D44">
-        <v>40</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="5"/>
-        <v>13.333333333333334</v>
+        <v>35</v>
+      </c>
+      <c r="E44" s="6">
+        <f t="shared" si="11"/>
+        <v>0.11666666666666667</v>
       </c>
       <c r="F44">
-        <v>13</v>
-      </c>
-      <c r="G44">
-        <f t="shared" si="6"/>
-        <v>5.6034482758620694</v>
+        <v>14</v>
+      </c>
+      <c r="G44" s="5">
+        <f t="shared" si="12"/>
+        <v>6.0344827586206899E-2</v>
       </c>
       <c r="H44" t="b">
         <v>0</v>
       </c>
       <c r="I44">
-        <v>249.50530092899999</v>
+        <v>31.9490138952</v>
       </c>
       <c r="J44">
-        <f t="shared" si="4"/>
-        <v>4.0079308787293591E-3</v>
+        <f t="shared" si="10"/>
+        <v>3.1299870577546664E-2</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="B45" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C45" s="5">
+        <f t="shared" si="9"/>
+        <v>4.7471264367816096E-2</v>
       </c>
       <c r="D45">
-        <v>20</v>
-      </c>
-      <c r="E45">
-        <f t="shared" si="5"/>
-        <v>6.666666666666667</v>
+        <v>22</v>
+      </c>
+      <c r="E45" s="6">
+        <f t="shared" si="11"/>
+        <v>7.3333333333333334E-2</v>
       </c>
       <c r="F45">
-        <v>5</v>
-      </c>
-      <c r="G45">
-        <f t="shared" si="6"/>
-        <v>2.1551724137931036</v>
+        <v>6</v>
+      </c>
+      <c r="G45" s="5">
+        <f t="shared" si="12"/>
+        <v>2.5862068965517241E-2</v>
       </c>
       <c r="H45" t="b">
         <v>0</v>
       </c>
       <c r="I45">
-        <v>66.643996215300007</v>
+        <v>45.634076474300002</v>
       </c>
       <c r="J45">
-        <f t="shared" si="4"/>
-        <v>1.5005102586726661E-2</v>
+        <f t="shared" si="10"/>
+        <v>2.1913448836050745E-2</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="B46" t="s">
-        <v>55</v>
+        <v>46</v>
+      </c>
+      <c r="C46" s="5">
+        <f t="shared" si="9"/>
+        <v>6.7701149425287349E-2</v>
       </c>
       <c r="D46">
-        <v>7</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="5"/>
-        <v>2.3333333333333335</v>
+        <v>41</v>
+      </c>
+      <c r="E46" s="6">
+        <f t="shared" si="11"/>
+        <v>0.13666666666666666</v>
       </c>
       <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="G46" s="5">
+        <f t="shared" si="12"/>
+        <v>6.8965517241379309E-2</v>
       </c>
       <c r="H46" t="b">
         <v>0</v>
       </c>
       <c r="I46">
-        <v>53.645178920799999</v>
+        <v>69.070577354500003</v>
       </c>
       <c r="J46">
-        <f t="shared" si="4"/>
-        <v>1.8641004096125163E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="B47" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47">
-        <v>38</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="5"/>
-        <v>12.666666666666668</v>
-      </c>
-      <c r="F47">
-        <v>15</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="6"/>
-        <v>6.4655172413793105</v>
-      </c>
-      <c r="H47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <v>49.728274775199999</v>
-      </c>
-      <c r="J47">
-        <f t="shared" si="4"/>
-        <v>2.0109283994278245E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="B48" t="s">
-        <v>57</v>
-      </c>
-      <c r="D48">
-        <v>5</v>
-      </c>
-      <c r="E48">
-        <f t="shared" si="5"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H48" t="b">
-        <v>0</v>
-      </c>
-      <c r="I48">
-        <v>21.3792568876</v>
-      </c>
-      <c r="J48">
-        <f t="shared" si="4"/>
-        <v>4.6774310503748209E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="B49" t="s">
-        <v>58</v>
-      </c>
-      <c r="D49">
-        <v>5</v>
-      </c>
-      <c r="E49">
-        <f t="shared" si="5"/>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-      <c r="G49">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H49" t="b">
-        <v>0</v>
-      </c>
-      <c r="I49">
-        <v>21.3792568876</v>
-      </c>
-      <c r="J49">
-        <f t="shared" si="4"/>
-        <v>4.6774310503748209E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+        <f>1/I46</f>
+        <v>1.4477944709620256E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D54">
         <v>5</v>
@@ -2276,10 +2343,10 @@
         <v>62117.036675900003</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:9">
       <c r="A55" s="1"/>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D55">
         <v>2</v>
@@ -2291,9 +2358,9 @@
         <v>1672.6144026500001</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:9">
       <c r="B56" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D56">
         <v>2</v>
@@ -2305,9 +2372,9 @@
         <v>1672.6144026500001</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:9">
       <c r="B57" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -2319,9 +2386,9 @@
         <v>1672.6144026500001</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:9">
       <c r="B58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D58">
         <v>3</v>
@@ -2333,9 +2400,9 @@
         <v>1063.3154804400001</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:9">
       <c r="B59" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D59">
         <v>2</v>
@@ -2347,9 +2414,9 @@
         <v>727.79310185600002</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:9">
       <c r="B60" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D60">
         <v>3</v>
@@ -2361,9 +2428,9 @@
         <v>602.05849959</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:9">
       <c r="B61" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -2375,9 +2442,9 @@
         <v>345.964830818</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:9">
       <c r="B62" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D62">
         <v>2</v>
@@ -2389,9 +2456,9 @@
         <v>345.964830818</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:9">
       <c r="B63" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D63">
         <v>2</v>
@@ -2403,7 +2470,7 @@
         <v>177.70821317400001</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:9">
       <c r="B64" t="s">
         <v>6</v>
       </c>
@@ -2419,7 +2486,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="B65" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D65">
         <v>3</v>
@@ -2433,7 +2500,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="B66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D66">
         <v>20</v>
@@ -2447,7 +2514,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="B67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D67">
         <v>7</v>
@@ -2461,10 +2528,10 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D68">
         <v>28</v>
@@ -2478,7 +2545,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="B69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D69">
         <v>26</v>
@@ -2492,7 +2559,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="B70" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D70">
         <v>25</v>
@@ -2506,7 +2573,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="B71" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D71">
         <v>44</v>
@@ -2520,7 +2587,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="B72" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D72">
         <v>17</v>
@@ -2534,7 +2601,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="B73" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D73">
         <v>16</v>
@@ -2548,7 +2615,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="B74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D74">
         <v>16</v>
@@ -2562,7 +2629,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="B75" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D75">
         <v>13</v>
@@ -2576,7 +2643,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="B76" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D76">
         <v>13</v>
@@ -2590,7 +2657,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="B77" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D77">
         <v>51</v>
@@ -2604,7 +2671,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="B78" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D78">
         <v>11</v>
@@ -2618,7 +2685,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="B79" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D79">
         <v>106</v>
@@ -2632,7 +2699,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="B80" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D80">
         <v>259</v>
@@ -2660,7 +2727,7 @@
     </row>
     <row r="82" spans="1:10">
       <c r="B82" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D82">
         <v>8</v>
@@ -2674,7 +2741,7 @@
     </row>
     <row r="83" spans="1:10">
       <c r="B83" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D83">
         <v>8</v>
@@ -2688,7 +2755,7 @@
     </row>
     <row r="84" spans="1:10">
       <c r="B84" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D84">
         <v>8</v>
@@ -2702,7 +2769,7 @@
     </row>
     <row r="85" spans="1:10">
       <c r="B85" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D85">
         <v>8</v>
@@ -2716,7 +2783,7 @@
     </row>
     <row r="86" spans="1:10">
       <c r="B86" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D86">
         <v>363</v>
@@ -2730,7 +2797,7 @@
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B91">
         <v>159</v>
@@ -2760,7 +2827,7 @@
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="1" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B95">
         <v>79</v>
@@ -2768,7 +2835,7 @@
     </row>
     <row r="96" spans="1:10">
       <c r="B96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D96">
         <v>24</v>
@@ -2794,85 +2861,85 @@
     </row>
     <row r="97" spans="1:10">
       <c r="B97" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D97">
         <v>9</v>
       </c>
       <c r="E97">
-        <f t="shared" ref="E97:E99" si="7">D97/$B$95*100</f>
+        <f t="shared" ref="E97:E99" si="13">D97/$B$95*100</f>
         <v>11.39240506329114</v>
       </c>
       <c r="F97">
         <v>5</v>
       </c>
       <c r="G97">
-        <f t="shared" ref="G97:G99" si="8">F97/$B$91*100</f>
+        <f t="shared" ref="G97:G99" si="14">F97/$B$91*100</f>
         <v>3.1446540880503147</v>
       </c>
       <c r="I97">
         <v>74.114175263800007</v>
       </c>
       <c r="J97">
-        <f t="shared" ref="J97:J99" si="9">1/I97</f>
+        <f t="shared" ref="J97:J99" si="15">1/I97</f>
         <v>1.3492695512574036E-2</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="B98" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D98">
         <v>56</v>
       </c>
       <c r="E98">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>70.886075949367083</v>
       </c>
       <c r="F98">
         <v>73</v>
       </c>
       <c r="G98">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>45.911949685534594</v>
       </c>
       <c r="I98">
         <v>72.859334163900002</v>
       </c>
       <c r="J98">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1.3725077390227857E-2</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="B99" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D99">
         <v>34</v>
       </c>
       <c r="E99">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>43.037974683544306</v>
       </c>
       <c r="F99">
         <v>42</v>
       </c>
       <c r="G99">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>26.415094339622641</v>
       </c>
       <c r="I99">
         <v>30.679398791899999</v>
       </c>
       <c r="J99">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>3.2595162857755246E-2</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="1" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B102">
         <v>272</v>
@@ -2880,7 +2947,7 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="1" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B103">
         <v>29</v>
@@ -2888,7 +2955,7 @@
     </row>
     <row r="104" spans="1:10">
       <c r="B104" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D104">
         <v>12</v>
@@ -2910,7 +2977,7 @@
     </row>
     <row r="105" spans="1:10">
       <c r="B105" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="D105">
         <v>9</v>
@@ -2931,8 +2998,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B15:K26">
-    <sortCondition ref="J15:J26"/>
+  <sortState ref="A33:X37">
+    <sortCondition ref="J33:J37"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>